<commit_message>
Add the ability to specify state of sample during import, project age unit and date received field to sample for cpgr
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/test.xlsx
+++ b/baobab/lims/setupdata/test/test.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="1104">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -2445,12 +2445,18 @@
     <t xml:space="preserve">SampleType</t>
   </si>
   <si>
+    <t xml:space="preserve">SampleState</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biospecimens</t>
   </si>
   <si>
     <t xml:space="preserve">Linked Sample</t>
   </si>
   <si>
+    <t xml:space="preserve">Sample State: register, due or received(default)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 1</t>
   </si>
   <si>
@@ -2466,6 +2472,9 @@
     <t xml:space="preserve">ml</t>
   </si>
   <si>
+    <t xml:space="preserve">due</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 2</t>
   </si>
   <si>
@@ -2490,6 +2499,9 @@
     <t xml:space="preserve">Def 003</t>
   </si>
   <si>
+    <t xml:space="preserve">Due</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 4</t>
   </si>
   <si>
@@ -2521,6 +2533,9 @@
   </si>
   <si>
     <t xml:space="preserve">Def 006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
   </si>
   <si>
     <t xml:space="preserve">Setup – Global defaults</t>
@@ -3455,7 +3470,7 @@
     <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="171" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3694,6 +3709,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3774,7 +3796,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4425,6 +4447,10 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -4580,7 +4606,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.19028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="110.866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="6.85425101214575"/>
   </cols>
   <sheetData>
@@ -4650,7 +4676,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.3886639676113"/>
@@ -4968,9 +4994,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="21" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -5245,11 +5271,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -5422,9 +5448,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5492,7 +5518,7 @@
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5637,12 +5663,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
@@ -5910,11 +5936,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6015,9 +6041,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6108,11 +6134,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -6621,10 +6647,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -6694,12 +6720,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
@@ -7050,8 +7076,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7101,8 +7127,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7155,7 +7181,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -7275,7 +7301,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
@@ -7446,9 +7472,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.3076923076923"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -7525,7 +7551,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -7898,16 +7924,18 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7981,7 +8009,7 @@
         <v>596</v>
       </c>
       <c r="C4" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D4" s="89" t="s">
         <v>597</v>
@@ -8005,7 +8033,7 @@
         <v>601</v>
       </c>
       <c r="C5" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D5" s="89" t="s">
         <v>602</v>
@@ -8029,7 +8057,7 @@
         <v>606</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D6" s="89" t="s">
         <v>607</v>
@@ -8053,7 +8081,7 @@
         <v>611</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D7" s="89" t="s">
         <v>612</v>
@@ -8077,7 +8105,7 @@
         <v>616</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D8" s="89" t="s">
         <v>617</v>
@@ -8101,7 +8129,7 @@
         <v>621</v>
       </c>
       <c r="C9" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D9" s="89" t="s">
         <v>622</v>
@@ -8142,10 +8170,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="61.4858299595142"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="96" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8319,8 +8347,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -8391,26 +8419,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8680,8 +8708,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -9075,18 +9103,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="44.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9237,17 +9265,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9390,9 +9418,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -9492,15 +9520,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.7408906882591"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -9671,12 +9699,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="6.42914979757085"/>
   </cols>
   <sheetData>
@@ -9809,23 +9837,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9874,10 +9905,13 @@
       <c r="O1" s="6" t="s">
         <v>764</v>
       </c>
+      <c r="P1" s="6" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="94" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -9935,15 +9969,18 @@
         <v>430</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>769</v>
+      </c>
+      <c r="P3" s="163" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="C4" s="79" t="s">
         <v>433</v>
@@ -9953,30 +9990,33 @@
       </c>
       <c r="E4" s="79"/>
       <c r="F4" s="88" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="G4" s="89"/>
       <c r="H4" s="89" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L4" s="93"/>
       <c r="N4" s="40" t="s">
         <v>178</v>
       </c>
       <c r="O4" s="40"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P4" s="0" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="C5" s="79" t="s">
         <v>433</v>
@@ -9986,30 +10026,33 @@
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="88" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="G5" s="89"/>
       <c r="H5" s="89" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L5" s="93"/>
       <c r="N5" s="40" t="s">
         <v>178</v>
       </c>
       <c r="O5" s="40"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P5" s="0" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="C6" s="79" t="s">
         <v>433</v>
@@ -10019,30 +10062,33 @@
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="88" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="G6" s="89"/>
       <c r="H6" s="89" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>30</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L6" s="93"/>
       <c r="N6" s="40" t="s">
         <v>172</v>
       </c>
       <c r="O6" s="40"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P6" s="0" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="C7" s="79" t="s">
         <v>433</v>
@@ -10052,7 +10098,7 @@
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="88" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
       <c r="G7" s="89"/>
       <c r="H7" s="89"/>
@@ -10060,7 +10106,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L7" s="93"/>
       <c r="N7" s="40" t="s">
@@ -10068,12 +10114,12 @@
       </c>
       <c r="O7" s="40"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>433</v>
@@ -10083,15 +10129,17 @@
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="88" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="G8" s="89"/>
       <c r="H8" s="89" t="s">
-        <v>788</v>
-      </c>
-      <c r="I8" s="5"/>
+        <v>792</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>15</v>
+      </c>
       <c r="J8" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L8" s="93"/>
       <c r="N8" s="40" t="s">
@@ -10101,10 +10149,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="C9" s="79" t="s">
         <v>433</v>
@@ -10114,23 +10162,26 @@
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="88" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="G9" s="89"/>
       <c r="H9" s="89" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>10</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L9" s="93"/>
       <c r="N9" s="33" t="s">
         <v>165</v>
       </c>
       <c r="O9" s="40"/>
+      <c r="P9" s="0" t="s">
+        <v>797</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10157,10 +10208,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -10172,15 +10223,15 @@
       <c r="B1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="163" t="s">
+      <c r="C1" s="164" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="14" t="s">
-        <v>793</v>
-      </c>
-      <c r="C2" s="164"/>
+        <v>798</v>
+      </c>
+      <c r="C2" s="165"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
@@ -10189,73 +10240,73 @@
       <c r="B3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="163" t="s">
+      <c r="C3" s="164" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>794</v>
+        <v>799</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>795</v>
-      </c>
-      <c r="C4" s="165" t="n">
+        <v>800</v>
+      </c>
+      <c r="C4" s="166" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>797</v>
-      </c>
-      <c r="C5" s="165" t="n">
+        <v>802</v>
+      </c>
+      <c r="C5" s="166" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>798</v>
-      </c>
-      <c r="C6" s="165" t="s">
-        <v>799</v>
+        <v>803</v>
+      </c>
+      <c r="C6" s="166" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>800</v>
+        <v>805</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>801</v>
-      </c>
-      <c r="C7" s="166" t="n">
+        <v>806</v>
+      </c>
+      <c r="C7" s="167" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>803</v>
-      </c>
-      <c r="C8" s="166" t="n">
+        <v>808</v>
+      </c>
+      <c r="C8" s="167" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>805</v>
-      </c>
-      <c r="C9" s="165" t="n">
+        <v>810</v>
+      </c>
+      <c r="C9" s="166" t="n">
         <v>15</v>
       </c>
     </row>
@@ -10264,240 +10315,240 @@
         <v>498</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>806</v>
-      </c>
-      <c r="C10" s="165" t="n">
+        <v>811</v>
+      </c>
+      <c r="C10" s="166" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>808</v>
-      </c>
-      <c r="C11" s="165" t="n">
+        <v>813</v>
+      </c>
+      <c r="C11" s="166" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>809</v>
+        <v>814</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>810</v>
-      </c>
-      <c r="C12" s="165" t="n">
+        <v>815</v>
+      </c>
+      <c r="C12" s="166" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>811</v>
+        <v>816</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>812</v>
-      </c>
-      <c r="C13" s="165" t="n">
+        <v>817</v>
+      </c>
+      <c r="C13" s="166" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>814</v>
-      </c>
-      <c r="C14" s="165"/>
+        <v>819</v>
+      </c>
+      <c r="C14" s="166"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>816</v>
-      </c>
-      <c r="C15" s="166" t="n">
+        <v>821</v>
+      </c>
+      <c r="C15" s="167" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>818</v>
-      </c>
-      <c r="C16" s="166" t="n">
+        <v>823</v>
+      </c>
+      <c r="C16" s="167" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>819</v>
+        <v>824</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>820</v>
-      </c>
-      <c r="C17" s="166" t="n">
+        <v>825</v>
+      </c>
+      <c r="C17" s="167" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>822</v>
-      </c>
-      <c r="C18" s="167" t="s">
-        <v>823</v>
-      </c>
-      <c r="D18" s="168"/>
+        <v>827</v>
+      </c>
+      <c r="C18" s="168" t="s">
+        <v>828</v>
+      </c>
+      <c r="D18" s="169"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>824</v>
+        <v>829</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>825</v>
-      </c>
-      <c r="C19" s="169" t="s">
+        <v>830</v>
+      </c>
+      <c r="C19" s="170" t="s">
         <v>301</v>
       </c>
-      <c r="D19" s="168"/>
+      <c r="D19" s="169"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>826</v>
+        <v>831</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>827</v>
-      </c>
-      <c r="C20" s="169" t="s">
+        <v>832</v>
+      </c>
+      <c r="C20" s="170" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>829</v>
-      </c>
-      <c r="C21" s="167" t="n">
+        <v>834</v>
+      </c>
+      <c r="C21" s="168" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>831</v>
-      </c>
-      <c r="C22" s="167" t="n">
+        <v>836</v>
+      </c>
+      <c r="C22" s="168" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>833</v>
-      </c>
-      <c r="C23" s="167" t="n">
+        <v>838</v>
+      </c>
+      <c r="C23" s="168" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>835</v>
-      </c>
-      <c r="C24" s="169" t="s">
-        <v>836</v>
-      </c>
-      <c r="D24" s="170"/>
+        <v>840</v>
+      </c>
+      <c r="C24" s="170" t="s">
+        <v>841</v>
+      </c>
+      <c r="D24" s="171"/>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>838</v>
-      </c>
-      <c r="C25" s="169" t="s">
-        <v>839</v>
+        <v>843</v>
+      </c>
+      <c r="C25" s="170" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>840</v>
+        <v>845</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>841</v>
-      </c>
-      <c r="C26" s="166" t="n">
+        <v>846</v>
+      </c>
+      <c r="C26" s="167" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>843</v>
-      </c>
-      <c r="C27" s="165" t="s">
+        <v>848</v>
+      </c>
+      <c r="C27" s="166" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>845</v>
-      </c>
-      <c r="C28" s="165" t="n">
+        <v>850</v>
+      </c>
+      <c r="C28" s="166" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>846</v>
+        <v>851</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>847</v>
-      </c>
-      <c r="C29" s="166" t="n">
+        <v>852</v>
+      </c>
+      <c r="C29" s="167" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>848</v>
+        <v>853</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>849</v>
-      </c>
-      <c r="C30" s="165"/>
+        <v>854</v>
+      </c>
+      <c r="C30" s="166"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>850</v>
+        <v>855</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>851</v>
-      </c>
-      <c r="C31" s="171" t="s">
-        <v>852</v>
+        <v>856</v>
+      </c>
+      <c r="C31" s="172" t="s">
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -10636,35 +10687,35 @@
   </cols>
   <sheetData>
     <row r="1" s="31" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="173" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="172" t="s">
+      <c r="B1" s="173" t="s">
         <v>198</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>855</v>
+        <v>860</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>856</v>
-      </c>
-      <c r="G1" s="173" t="s">
-        <v>857</v>
+        <v>861</v>
+      </c>
+      <c r="G1" s="174" t="s">
+        <v>862</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>858</v>
+        <v>863</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>859</v>
+        <v>864</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>860</v>
+        <v>865</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>511</v>
@@ -10679,63 +10730,63 @@
         <v>243</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>861</v>
-      </c>
-      <c r="E2" s="174" t="s">
-        <v>862</v>
+        <v>866</v>
+      </c>
+      <c r="E2" s="175" t="s">
+        <v>867</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>863</v>
+        <v>868</v>
       </c>
       <c r="G2" s="51" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>864</v>
+        <v>869</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>865</v>
+        <v>870</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>866</v>
+        <v>871</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>868</v>
+        <v>873</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>869</v>
+        <v>874</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>301</v>
       </c>
-      <c r="E3" s="174" t="s">
-        <v>839</v>
+      <c r="E3" s="175" t="s">
+        <v>844</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>870</v>
+        <v>875</v>
       </c>
       <c r="G3" s="51" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="51" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="K3" s="51" t="s">
         <v>535</v>
@@ -10743,51 +10794,51 @@
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>225</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>836</v>
-      </c>
-      <c r="G4" s="174"/>
+        <v>841</v>
+      </c>
+      <c r="G4" s="175"/>
       <c r="H4" s="51" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>878</v>
-      </c>
-      <c r="G5" s="174"/>
+        <v>883</v>
+      </c>
+      <c r="G5" s="175"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>880</v>
-      </c>
-      <c r="G6" s="174"/>
+        <v>885</v>
+      </c>
+      <c r="G6" s="175"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>881</v>
+        <v>886</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>882</v>
-      </c>
-      <c r="G7" s="174"/>
+        <v>887</v>
+      </c>
+      <c r="G7" s="175"/>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
@@ -10796,108 +10847,108 @@
       <c r="B8" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="G8" s="174"/>
+      <c r="G8" s="175"/>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="174"/>
+      <c r="G9" s="175"/>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="174"/>
+      <c r="G10" s="175"/>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="174"/>
+      <c r="G11" s="175"/>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="174"/>
+      <c r="G12" s="175"/>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="174"/>
+      <c r="G13" s="175"/>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="174"/>
+      <c r="G14" s="175"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="174"/>
+      <c r="G15" s="175"/>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="174"/>
+      <c r="G16" s="175"/>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="174"/>
+      <c r="G17" s="175"/>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="174"/>
+      <c r="G18" s="175"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="174"/>
+      <c r="G19" s="175"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="175"/>
-      <c r="B20" s="175"/>
-      <c r="C20" s="175"/>
-      <c r="D20" s="175"/>
-      <c r="E20" s="176"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="175"/>
-      <c r="I20" s="175"/>
-      <c r="J20" s="175"/>
-      <c r="K20" s="175"/>
-      <c r="L20" s="175"/>
-    </row>
-    <row r="21" s="178" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="176"/>
+      <c r="B20" s="176"/>
+      <c r="C20" s="176"/>
+      <c r="D20" s="176"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="176"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="176"/>
+      <c r="I20" s="176"/>
+      <c r="J20" s="176"/>
+      <c r="K20" s="176"/>
+      <c r="L20" s="176"/>
+    </row>
+    <row r="21" s="179" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>883</v>
+        <v>888</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>884</v>
+        <v>889</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>885</v>
-      </c>
-      <c r="E21" s="177" t="s">
-        <v>886</v>
+        <v>890</v>
+      </c>
+      <c r="E21" s="178" t="s">
+        <v>891</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>887</v>
+        <v>892</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>888</v>
+        <v>893</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>889</v>
+        <v>894</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>890</v>
+        <v>895</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="179" t="s">
-        <v>891</v>
+      <c r="A22" s="180" t="s">
+        <v>896</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>892</v>
+        <v>897</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>893</v>
+        <v>898</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>894</v>
-      </c>
-      <c r="E22" s="174" t="s">
-        <v>895</v>
+        <v>899</v>
+      </c>
+      <c r="E22" s="175" t="s">
+        <v>900</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>896</v>
+        <v>901</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="H22" s="51" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="I22" s="51" t="s">
         <v>520</v>
@@ -10905,970 +10956,970 @@
     </row>
     <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="51" t="s">
-        <v>898</v>
+        <v>903</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>899</v>
+        <v>904</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>900</v>
-      </c>
-      <c r="E23" s="174" t="s">
-        <v>901</v>
+        <v>905</v>
+      </c>
+      <c r="E23" s="175" t="s">
+        <v>906</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="G23" s="51" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>904</v>
+        <v>909</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="51" t="s">
-        <v>905</v>
+        <v>910</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>907</v>
+        <v>912</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>908</v>
+        <v>913</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>909</v>
+        <v>914</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>909</v>
+        <v>914</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="51" t="s">
-        <v>911</v>
+        <v>916</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>912</v>
+        <v>917</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="H25" s="51" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="51" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>917</v>
+        <v>922</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>918</v>
+        <v>923</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="51" t="s">
-        <v>919</v>
+        <v>924</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>920</v>
+        <v>925</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="51" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>922</v>
+        <v>927</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="51" t="s">
-        <v>923</v>
+        <v>928</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>924</v>
+        <v>929</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="51" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="51" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>928</v>
+        <v>933</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="51" t="s">
-        <v>929</v>
+        <v>934</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>930</v>
+        <v>935</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="51" t="s">
-        <v>931</v>
+        <v>936</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>932</v>
+        <v>937</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="51" t="s">
-        <v>933</v>
+        <v>938</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="51" t="s">
-        <v>934</v>
+        <v>939</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="51" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="51" t="s">
-        <v>936</v>
+        <v>941</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="51" t="s">
-        <v>937</v>
+        <v>942</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="51" t="s">
-        <v>938</v>
+        <v>943</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="51" t="s">
-        <v>939</v>
+        <v>944</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="51" t="s">
-        <v>940</v>
+        <v>945</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="51" t="s">
-        <v>941</v>
+        <v>946</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="51" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="51" t="s">
-        <v>943</v>
+        <v>948</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="51" t="s">
-        <v>944</v>
+        <v>949</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="51" t="s">
-        <v>945</v>
+        <v>950</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="51" t="s">
-        <v>946</v>
+        <v>951</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="51" t="s">
-        <v>947</v>
+        <v>952</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="51" t="s">
-        <v>948</v>
+        <v>953</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="51" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="51" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="51" t="s">
-        <v>951</v>
+        <v>956</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="51" t="s">
-        <v>952</v>
+        <v>957</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="51" t="s">
-        <v>953</v>
+        <v>958</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="51" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="51" t="s">
-        <v>955</v>
+        <v>960</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="51" t="s">
-        <v>956</v>
+        <v>961</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="51" t="s">
-        <v>957</v>
+        <v>962</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="51" t="s">
-        <v>958</v>
+        <v>963</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="51" t="s">
-        <v>959</v>
+        <v>964</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="51" t="s">
-        <v>960</v>
+        <v>965</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="51" t="s">
-        <v>961</v>
+        <v>966</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="51" t="s">
-        <v>962</v>
+        <v>967</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="51" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="51" t="s">
-        <v>964</v>
+        <v>969</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="51" t="s">
-        <v>965</v>
+        <v>970</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="51" t="s">
-        <v>966</v>
+        <v>971</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="51" t="s">
-        <v>967</v>
+        <v>972</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="51" t="s">
-        <v>968</v>
+        <v>973</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="51" t="s">
-        <v>969</v>
+        <v>974</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="51" t="s">
-        <v>970</v>
+        <v>975</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="51" t="s">
-        <v>971</v>
+        <v>976</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="51" t="s">
-        <v>972</v>
+        <v>977</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="51" t="s">
-        <v>973</v>
+        <v>978</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="51" t="s">
-        <v>974</v>
+        <v>979</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="51" t="s">
-        <v>975</v>
+        <v>980</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="51" t="s">
-        <v>976</v>
+        <v>981</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="51" t="s">
-        <v>977</v>
+        <v>982</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="51" t="s">
-        <v>978</v>
+        <v>983</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="51" t="s">
-        <v>979</v>
+        <v>984</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="51" t="s">
-        <v>980</v>
+        <v>985</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="51" t="s">
-        <v>981</v>
+        <v>986</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="51" t="s">
-        <v>982</v>
+        <v>987</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="51" t="s">
-        <v>983</v>
+        <v>988</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="51" t="s">
-        <v>984</v>
+        <v>989</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="51" t="s">
-        <v>985</v>
+        <v>990</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="51" t="s">
-        <v>986</v>
+        <v>991</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="51" t="s">
-        <v>987</v>
+        <v>992</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="51" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="51" t="s">
-        <v>989</v>
+        <v>994</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="51" t="s">
-        <v>990</v>
+        <v>995</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="51" t="s">
-        <v>991</v>
+        <v>996</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="51" t="s">
-        <v>992</v>
+        <v>997</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="51" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="51" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="51" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="51" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="51" t="s">
-        <v>997</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="51" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="51" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="51" t="s">
-        <v>1000</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="51" t="s">
-        <v>1001</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="51" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="51" t="s">
-        <v>1003</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="51" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="51" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="51" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="51" t="s">
-        <v>1007</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="51" t="s">
-        <v>1008</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="51" t="s">
-        <v>1009</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="51" t="s">
-        <v>1010</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="51" t="s">
-        <v>1011</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="51" t="s">
-        <v>1012</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="51" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="51" t="s">
-        <v>1014</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="51" t="s">
-        <v>1015</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="51" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="51" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="51" t="s">
-        <v>1018</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="51" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="51" t="s">
-        <v>1020</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="51" t="s">
-        <v>1021</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="51" t="s">
-        <v>1022</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="51" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="51" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="51" t="s">
-        <v>1025</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="51" t="s">
-        <v>1026</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="51" t="s">
-        <v>1027</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="51" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="51" t="s">
-        <v>1029</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="51" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="51" t="s">
-        <v>1031</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="51" t="s">
-        <v>1032</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="51" t="s">
-        <v>1033</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="51" t="s">
-        <v>1034</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="51" t="s">
-        <v>1035</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="51" t="s">
-        <v>1036</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="51" t="s">
-        <v>1037</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="51" t="s">
-        <v>1038</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="51" t="s">
-        <v>1039</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="51" t="s">
-        <v>1040</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="51" t="s">
-        <v>1041</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="51" t="s">
-        <v>1042</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="51" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="51" t="s">
-        <v>1044</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="51" t="s">
-        <v>1045</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="51" t="s">
-        <v>1046</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="51" t="s">
-        <v>1047</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="51" t="s">
-        <v>1048</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="51" t="s">
-        <v>1049</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="51" t="s">
-        <v>1050</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="51" t="s">
-        <v>1051</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="51" t="s">
-        <v>1052</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="51" t="s">
-        <v>1053</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="51" t="s">
-        <v>1054</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="51" t="s">
-        <v>1055</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="51" t="s">
-        <v>1056</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="51" t="s">
-        <v>1057</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="51" t="s">
-        <v>1058</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="51" t="s">
-        <v>1059</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="51" t="s">
-        <v>1060</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="51" t="s">
-        <v>1061</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="51" t="s">
-        <v>1062</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="51" t="s">
-        <v>1063</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="51" t="s">
-        <v>1064</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="51" t="s">
-        <v>1065</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="51" t="s">
-        <v>1066</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="51" t="s">
-        <v>1067</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="51" t="s">
-        <v>1068</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="51" t="s">
-        <v>1069</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="51" t="s">
-        <v>1070</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="51" t="s">
-        <v>1071</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="51" t="s">
-        <v>1072</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="51" t="s">
-        <v>1073</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="51" t="s">
-        <v>1074</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="51" t="s">
-        <v>1075</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="51" t="s">
-        <v>1076</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="51" t="s">
-        <v>1077</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="51" t="s">
-        <v>1078</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="51" t="s">
-        <v>1079</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="51" t="s">
-        <v>1080</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="51" t="s">
-        <v>1081</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="51" t="s">
-        <v>1082</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="51" t="s">
-        <v>1083</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="51" t="s">
-        <v>1084</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="51" t="s">
-        <v>1085</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="51" t="s">
-        <v>1086</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="51" t="s">
-        <v>1087</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="51" t="s">
-        <v>1088</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="51" t="s">
-        <v>1089</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="51" t="s">
-        <v>1090</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="51" t="s">
-        <v>1091</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="51" t="s">
-        <v>1092</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="51" t="s">
-        <v>1093</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="51" t="s">
-        <v>1094</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="51" t="s">
-        <v>1095</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="51" t="s">
-        <v>1096</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="51" t="s">
-        <v>799</v>
+        <v>804</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="51" t="s">
-        <v>1097</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="51" t="s">
-        <v>1098</v>
+        <v>1103</v>
       </c>
     </row>
   </sheetData>
@@ -11897,10 +11948,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="28" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -12072,7 +12123,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74898785425101"/>
@@ -12276,10 +12327,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -12436,16 +12487,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -12915,13 +12966,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
@@ -13280,14 +13331,13 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
Custom template, javascript and sample processes for sample shipment
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/test.xlsx
+++ b/baobab/lims/setupdata/test/test.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1114">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -2521,6 +2521,51 @@
   </si>
   <si>
     <t xml:space="preserve">Def 006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Sample 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test sample 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Def 007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Sample 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test sample 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Sample 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test sample 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Def 009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Sample 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test sample 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Def 010</t>
   </si>
   <si>
     <t xml:space="preserve">Setup – Global defaults</t>
@@ -4580,7 +4625,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.19028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="106.153846153846"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="6.85425101214575"/>
   </cols>
   <sheetData>
@@ -4650,7 +4695,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.3886639676113"/>
@@ -4968,9 +5013,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="10" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="21" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -5245,11 +5290,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -5422,9 +5467,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5492,7 +5537,7 @@
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5637,12 +5682,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
@@ -5910,11 +5955,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6015,9 +6060,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6108,11 +6153,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -6621,10 +6666,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -6694,12 +6739,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
@@ -7050,8 +7095,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7101,8 +7146,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7155,7 +7200,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -7275,7 +7320,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5263157894737"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
@@ -7446,9 +7491,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -7525,7 +7570,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -7904,9 +7949,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
@@ -8142,10 +8187,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="61.4858299595142"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="96" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8319,8 +8364,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -8391,26 +8436,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8680,8 +8725,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -9075,18 +9120,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9237,17 +9282,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9390,9 +9435,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -9492,15 +9537,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.4574898785425"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -9671,12 +9716,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="6.42914979757085"/>
   </cols>
   <sheetData>
@@ -9809,22 +9854,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.8866396761134"/>
     <col collapsed="false" hidden="false" max="13" min="7" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
@@ -10131,6 +10176,134 @@
         <v>165</v>
       </c>
       <c r="O9" s="40"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="C10" s="79" t="s">
+        <v>433</v>
+      </c>
+      <c r="D10" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="79"/>
+      <c r="F10" s="88" t="s">
+        <v>795</v>
+      </c>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89" t="s">
+        <v>796</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="L10" s="93"/>
+      <c r="N10" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="O10" s="40"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>797</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>798</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>433</v>
+      </c>
+      <c r="D11" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="79"/>
+      <c r="F11" s="88" t="s">
+        <v>799</v>
+      </c>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="L11" s="93"/>
+      <c r="N11" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="O11" s="40"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>800</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>801</v>
+      </c>
+      <c r="C12" s="79" t="s">
+        <v>433</v>
+      </c>
+      <c r="D12" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="79"/>
+      <c r="F12" s="88" t="s">
+        <v>802</v>
+      </c>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89" t="s">
+        <v>803</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="L12" s="93"/>
+      <c r="N12" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="O12" s="40"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>805</v>
+      </c>
+      <c r="C13" s="79" t="s">
+        <v>433</v>
+      </c>
+      <c r="D13" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="79"/>
+      <c r="F13" s="88" t="s">
+        <v>806</v>
+      </c>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89" t="s">
+        <v>807</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="L13" s="93"/>
+      <c r="N13" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="O13" s="40"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10157,10 +10330,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -10178,7 +10351,7 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="14" t="s">
-        <v>793</v>
+        <v>808</v>
       </c>
       <c r="C2" s="164"/>
     </row>
@@ -10195,10 +10368,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>794</v>
+        <v>809</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>795</v>
+        <v>810</v>
       </c>
       <c r="C4" s="165" t="n">
         <v>0</v>
@@ -10206,10 +10379,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>796</v>
+        <v>811</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>797</v>
+        <v>812</v>
       </c>
       <c r="C5" s="165" t="n">
         <v>0</v>
@@ -10217,21 +10390,21 @@
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>798</v>
+        <v>813</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>798</v>
+        <v>813</v>
       </c>
       <c r="C6" s="165" t="s">
-        <v>799</v>
+        <v>814</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>800</v>
+        <v>815</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>801</v>
+        <v>816</v>
       </c>
       <c r="C7" s="166" t="n">
         <v>0</v>
@@ -10239,10 +10412,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>802</v>
+        <v>817</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>803</v>
+        <v>818</v>
       </c>
       <c r="C8" s="166" t="n">
         <v>1</v>
@@ -10250,10 +10423,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>804</v>
+        <v>819</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>805</v>
+        <v>820</v>
       </c>
       <c r="C9" s="165" t="n">
         <v>15</v>
@@ -10264,7 +10437,7 @@
         <v>498</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>806</v>
+        <v>821</v>
       </c>
       <c r="C10" s="165" t="n">
         <v>14</v>
@@ -10272,10 +10445,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>807</v>
+        <v>822</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>808</v>
+        <v>823</v>
       </c>
       <c r="C11" s="165" t="n">
         <v>5</v>
@@ -10283,10 +10456,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>809</v>
+        <v>824</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>810</v>
+        <v>825</v>
       </c>
       <c r="C12" s="165" t="n">
         <v>5</v>
@@ -10294,10 +10467,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>811</v>
+        <v>826</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>812</v>
+        <v>827</v>
       </c>
       <c r="C13" s="165" t="n">
         <v>4</v>
@@ -10305,19 +10478,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>813</v>
+        <v>828</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>814</v>
+        <v>829</v>
       </c>
       <c r="C14" s="165"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>815</v>
+        <v>830</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>816</v>
+        <v>831</v>
       </c>
       <c r="C15" s="166" t="n">
         <v>0</v>
@@ -10325,10 +10498,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>817</v>
+        <v>832</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>818</v>
+        <v>833</v>
       </c>
       <c r="C16" s="166" t="n">
         <v>0</v>
@@ -10336,10 +10509,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>819</v>
+        <v>834</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>820</v>
+        <v>835</v>
       </c>
       <c r="C17" s="166" t="n">
         <v>1</v>
@@ -10347,22 +10520,22 @@
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>821</v>
+        <v>836</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>822</v>
+        <v>837</v>
       </c>
       <c r="C18" s="167" t="s">
-        <v>823</v>
+        <v>838</v>
       </c>
       <c r="D18" s="168"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>824</v>
+        <v>839</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>825</v>
+        <v>840</v>
       </c>
       <c r="C19" s="169" t="s">
         <v>301</v>
@@ -10371,10 +10544,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>826</v>
+        <v>841</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>827</v>
+        <v>842</v>
       </c>
       <c r="C20" s="169" t="s">
         <v>301</v>
@@ -10382,10 +10555,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>828</v>
+        <v>843</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>829</v>
+        <v>844</v>
       </c>
       <c r="C21" s="167" t="n">
         <v>30</v>
@@ -10393,10 +10566,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>830</v>
+        <v>845</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>831</v>
+        <v>846</v>
       </c>
       <c r="C22" s="167" t="n">
         <v>0</v>
@@ -10404,10 +10577,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>832</v>
+        <v>847</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>833</v>
+        <v>848</v>
       </c>
       <c r="C23" s="167" t="n">
         <v>0</v>
@@ -10415,33 +10588,33 @@
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>834</v>
+        <v>849</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>835</v>
+        <v>850</v>
       </c>
       <c r="C24" s="169" t="s">
-        <v>836</v>
+        <v>851</v>
       </c>
       <c r="D24" s="170"/>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>837</v>
+        <v>852</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>838</v>
+        <v>853</v>
       </c>
       <c r="C25" s="169" t="s">
-        <v>839</v>
+        <v>854</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>840</v>
+        <v>855</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>841</v>
+        <v>856</v>
       </c>
       <c r="C26" s="166" t="n">
         <v>0</v>
@@ -10449,10 +10622,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>842</v>
+        <v>857</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>843</v>
+        <v>858</v>
       </c>
       <c r="C27" s="165" t="s">
         <v>597</v>
@@ -10460,10 +10633,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>844</v>
+        <v>859</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>845</v>
+        <v>860</v>
       </c>
       <c r="C28" s="165" t="n">
         <v>2</v>
@@ -10471,10 +10644,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>846</v>
+        <v>861</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>847</v>
+        <v>862</v>
       </c>
       <c r="C29" s="166" t="n">
         <v>0</v>
@@ -10482,22 +10655,22 @@
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>848</v>
+        <v>863</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>849</v>
+        <v>864</v>
       </c>
       <c r="C30" s="165"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>850</v>
+        <v>865</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>851</v>
+        <v>866</v>
       </c>
       <c r="C31" s="171" t="s">
-        <v>852</v>
+        <v>867</v>
       </c>
     </row>
   </sheetData>
@@ -10643,28 +10816,28 @@
         <v>198</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>853</v>
+        <v>868</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>854</v>
+        <v>869</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>855</v>
+        <v>870</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>856</v>
+        <v>871</v>
       </c>
       <c r="G1" s="173" t="s">
-        <v>857</v>
+        <v>872</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>858</v>
+        <v>873</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>859</v>
+        <v>874</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>860</v>
+        <v>875</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>511</v>
@@ -10679,63 +10852,63 @@
         <v>243</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>823</v>
+        <v>838</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>861</v>
+        <v>876</v>
       </c>
       <c r="E2" s="174" t="s">
-        <v>862</v>
+        <v>877</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>863</v>
+        <v>878</v>
       </c>
       <c r="G2" s="51" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>864</v>
+        <v>879</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>865</v>
+        <v>880</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>866</v>
+        <v>881</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>867</v>
+        <v>882</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>868</v>
+        <v>883</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>869</v>
+        <v>884</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>301</v>
       </c>
       <c r="E3" s="174" t="s">
-        <v>839</v>
+        <v>854</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>870</v>
+        <v>885</v>
       </c>
       <c r="G3" s="51" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="51" t="s">
-        <v>871</v>
+        <v>886</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>872</v>
+        <v>887</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>873</v>
+        <v>888</v>
       </c>
       <c r="K3" s="51" t="s">
         <v>535</v>
@@ -10743,19 +10916,19 @@
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>874</v>
+        <v>889</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>225</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>875</v>
+        <v>890</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>876</v>
+        <v>891</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>836</v>
+        <v>851</v>
       </c>
       <c r="G4" s="174"/>
       <c r="H4" s="51" t="s">
@@ -10764,28 +10937,28 @@
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>877</v>
+        <v>892</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>878</v>
+        <v>893</v>
       </c>
       <c r="G5" s="174"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>879</v>
+        <v>894</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>880</v>
+        <v>895</v>
       </c>
       <c r="G6" s="174"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>881</v>
+        <v>896</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>882</v>
+        <v>897</v>
       </c>
       <c r="G7" s="174"/>
     </row>
@@ -10847,57 +11020,57 @@
     </row>
     <row r="21" s="178" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>883</v>
+        <v>898</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>798</v>
+        <v>813</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>884</v>
+        <v>899</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>885</v>
+        <v>900</v>
       </c>
       <c r="E21" s="177" t="s">
-        <v>886</v>
+        <v>901</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>887</v>
+        <v>902</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>888</v>
+        <v>903</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>889</v>
+        <v>904</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>890</v>
+        <v>905</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="179" t="s">
-        <v>891</v>
+        <v>906</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>892</v>
+        <v>907</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>893</v>
+        <v>908</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>894</v>
+        <v>909</v>
       </c>
       <c r="E22" s="174" t="s">
-        <v>895</v>
+        <v>910</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>896</v>
+        <v>911</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>897</v>
+        <v>912</v>
       </c>
       <c r="H22" s="51" t="s">
-        <v>897</v>
+        <v>912</v>
       </c>
       <c r="I22" s="51" t="s">
         <v>520</v>
@@ -10905,970 +11078,970 @@
     </row>
     <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="51" t="s">
-        <v>898</v>
+        <v>913</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>899</v>
+        <v>914</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>900</v>
+        <v>915</v>
       </c>
       <c r="E23" s="174" t="s">
-        <v>901</v>
+        <v>916</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>902</v>
+        <v>917</v>
       </c>
       <c r="G23" s="51" t="s">
-        <v>903</v>
+        <v>918</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>903</v>
+        <v>918</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>904</v>
+        <v>919</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="51" t="s">
-        <v>905</v>
+        <v>920</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>906</v>
+        <v>921</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>907</v>
+        <v>922</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>908</v>
+        <v>923</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>909</v>
+        <v>924</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>909</v>
+        <v>924</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>910</v>
+        <v>925</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="51" t="s">
-        <v>911</v>
+        <v>926</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>912</v>
+        <v>927</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>913</v>
+        <v>928</v>
       </c>
       <c r="H25" s="51" t="s">
-        <v>914</v>
+        <v>929</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>915</v>
+        <v>930</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="51" t="s">
-        <v>916</v>
+        <v>931</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>917</v>
+        <v>932</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>918</v>
+        <v>933</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="51" t="s">
-        <v>919</v>
+        <v>934</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>920</v>
+        <v>935</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="51" t="s">
-        <v>921</v>
+        <v>936</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>922</v>
+        <v>937</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="51" t="s">
-        <v>923</v>
+        <v>938</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>924</v>
+        <v>939</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="51" t="s">
-        <v>925</v>
+        <v>940</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>926</v>
+        <v>941</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="51" t="s">
-        <v>927</v>
+        <v>942</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>928</v>
+        <v>943</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="51" t="s">
-        <v>929</v>
+        <v>944</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>930</v>
+        <v>945</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="51" t="s">
-        <v>931</v>
+        <v>946</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>932</v>
+        <v>947</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="51" t="s">
-        <v>933</v>
+        <v>948</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="51" t="s">
-        <v>934</v>
+        <v>949</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="51" t="s">
-        <v>935</v>
+        <v>950</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="51" t="s">
-        <v>936</v>
+        <v>951</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="51" t="s">
-        <v>937</v>
+        <v>952</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="51" t="s">
-        <v>938</v>
+        <v>953</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="51" t="s">
-        <v>939</v>
+        <v>954</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="51" t="s">
-        <v>940</v>
+        <v>955</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="51" t="s">
-        <v>941</v>
+        <v>956</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="51" t="s">
-        <v>942</v>
+        <v>957</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="51" t="s">
-        <v>943</v>
+        <v>958</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="51" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="51" t="s">
-        <v>945</v>
+        <v>960</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="51" t="s">
-        <v>946</v>
+        <v>961</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="51" t="s">
-        <v>947</v>
+        <v>962</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="51" t="s">
-        <v>948</v>
+        <v>963</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="51" t="s">
-        <v>949</v>
+        <v>964</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="51" t="s">
-        <v>950</v>
+        <v>965</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="51" t="s">
-        <v>951</v>
+        <v>966</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="51" t="s">
-        <v>952</v>
+        <v>967</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="51" t="s">
-        <v>953</v>
+        <v>968</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="51" t="s">
-        <v>954</v>
+        <v>969</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="51" t="s">
-        <v>955</v>
+        <v>970</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="51" t="s">
-        <v>956</v>
+        <v>971</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="51" t="s">
-        <v>957</v>
+        <v>972</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="51" t="s">
-        <v>958</v>
+        <v>973</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="51" t="s">
-        <v>959</v>
+        <v>974</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="51" t="s">
-        <v>960</v>
+        <v>975</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="51" t="s">
-        <v>961</v>
+        <v>976</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="51" t="s">
-        <v>962</v>
+        <v>977</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="51" t="s">
-        <v>963</v>
+        <v>978</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="51" t="s">
-        <v>964</v>
+        <v>979</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="51" t="s">
-        <v>965</v>
+        <v>980</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="51" t="s">
-        <v>966</v>
+        <v>981</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="51" t="s">
-        <v>967</v>
+        <v>982</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="51" t="s">
-        <v>968</v>
+        <v>983</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="51" t="s">
-        <v>969</v>
+        <v>984</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="51" t="s">
-        <v>970</v>
+        <v>985</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="51" t="s">
-        <v>971</v>
+        <v>986</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="51" t="s">
-        <v>972</v>
+        <v>987</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="51" t="s">
-        <v>973</v>
+        <v>988</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="51" t="s">
-        <v>974</v>
+        <v>989</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="51" t="s">
-        <v>975</v>
+        <v>990</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="51" t="s">
-        <v>976</v>
+        <v>991</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="51" t="s">
-        <v>977</v>
+        <v>992</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="51" t="s">
-        <v>978</v>
+        <v>993</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="51" t="s">
-        <v>979</v>
+        <v>994</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="51" t="s">
-        <v>980</v>
+        <v>995</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="51" t="s">
-        <v>981</v>
+        <v>996</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="51" t="s">
-        <v>982</v>
+        <v>997</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="51" t="s">
-        <v>983</v>
+        <v>998</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="51" t="s">
-        <v>984</v>
+        <v>999</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="51" t="s">
-        <v>985</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="51" t="s">
-        <v>986</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="51" t="s">
-        <v>987</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="51" t="s">
-        <v>988</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="51" t="s">
-        <v>989</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="51" t="s">
-        <v>990</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="51" t="s">
-        <v>991</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="51" t="s">
-        <v>992</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="51" t="s">
-        <v>993</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="51" t="s">
-        <v>994</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="51" t="s">
-        <v>995</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="51" t="s">
-        <v>996</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="51" t="s">
-        <v>997</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="51" t="s">
-        <v>998</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="51" t="s">
-        <v>999</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="51" t="s">
-        <v>1000</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="51" t="s">
-        <v>1001</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="51" t="s">
-        <v>1002</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="51" t="s">
-        <v>1003</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="51" t="s">
-        <v>1004</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="51" t="s">
-        <v>1005</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="51" t="s">
-        <v>1006</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="51" t="s">
-        <v>1007</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="51" t="s">
-        <v>1008</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="51" t="s">
-        <v>1009</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="51" t="s">
-        <v>1010</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="51" t="s">
-        <v>1011</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="51" t="s">
-        <v>1012</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="51" t="s">
-        <v>1013</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="51" t="s">
-        <v>1014</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="51" t="s">
-        <v>1015</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="51" t="s">
-        <v>1016</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="51" t="s">
-        <v>1017</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="51" t="s">
-        <v>1018</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="51" t="s">
-        <v>1019</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="51" t="s">
-        <v>1020</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="51" t="s">
-        <v>1021</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="51" t="s">
-        <v>1022</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="51" t="s">
-        <v>1023</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="51" t="s">
-        <v>1024</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="51" t="s">
-        <v>1025</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="51" t="s">
-        <v>1026</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="51" t="s">
-        <v>1027</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="51" t="s">
-        <v>1028</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="51" t="s">
-        <v>1029</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="51" t="s">
-        <v>1030</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="51" t="s">
-        <v>1031</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="51" t="s">
-        <v>1032</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="51" t="s">
-        <v>1033</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="51" t="s">
-        <v>1034</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="51" t="s">
-        <v>1035</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="51" t="s">
-        <v>1036</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="51" t="s">
-        <v>1037</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="51" t="s">
-        <v>1038</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="51" t="s">
-        <v>1039</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="51" t="s">
-        <v>1040</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="51" t="s">
-        <v>1041</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="51" t="s">
-        <v>1042</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="51" t="s">
-        <v>1043</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="51" t="s">
-        <v>1044</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="51" t="s">
-        <v>1045</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="51" t="s">
-        <v>1046</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="51" t="s">
-        <v>1047</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="51" t="s">
-        <v>1048</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="51" t="s">
-        <v>1049</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="51" t="s">
-        <v>1050</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="51" t="s">
-        <v>1051</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="51" t="s">
-        <v>1052</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="51" t="s">
-        <v>1053</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="51" t="s">
-        <v>1054</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="51" t="s">
-        <v>1055</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="51" t="s">
-        <v>1056</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="51" t="s">
-        <v>1057</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="51" t="s">
-        <v>1058</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="51" t="s">
-        <v>1059</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="51" t="s">
-        <v>1060</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="51" t="s">
-        <v>1061</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="51" t="s">
-        <v>1062</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="51" t="s">
-        <v>1063</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="51" t="s">
-        <v>1064</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="51" t="s">
-        <v>1065</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="51" t="s">
-        <v>1066</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="51" t="s">
-        <v>1067</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="51" t="s">
-        <v>1068</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="51" t="s">
-        <v>1069</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="51" t="s">
-        <v>1070</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="51" t="s">
-        <v>1071</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="51" t="s">
-        <v>1072</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="51" t="s">
-        <v>1073</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="51" t="s">
-        <v>1074</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="51" t="s">
-        <v>1075</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="51" t="s">
-        <v>1076</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="51" t="s">
-        <v>1077</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="51" t="s">
-        <v>1078</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="51" t="s">
-        <v>1079</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="51" t="s">
-        <v>1080</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="51" t="s">
-        <v>1081</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="51" t="s">
-        <v>1082</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="51" t="s">
-        <v>1083</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="51" t="s">
-        <v>1084</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="51" t="s">
-        <v>1085</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="51" t="s">
-        <v>1086</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="51" t="s">
-        <v>1087</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="51" t="s">
-        <v>1088</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="51" t="s">
-        <v>1089</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="51" t="s">
-        <v>1090</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="51" t="s">
-        <v>1091</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="51" t="s">
-        <v>1092</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="51" t="s">
-        <v>1093</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="51" t="s">
-        <v>1094</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="51" t="s">
-        <v>1095</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="51" t="s">
-        <v>1096</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="51" t="s">
-        <v>799</v>
+        <v>814</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="51" t="s">
-        <v>1097</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="51" t="s">
-        <v>1098</v>
+        <v>1113</v>
       </c>
     </row>
   </sheetData>
@@ -11897,10 +12070,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="28" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -12072,7 +12245,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74898785425101"/>
@@ -12276,10 +12449,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -12436,16 +12609,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -12915,13 +13088,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
@@ -13280,14 +13453,13 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
Alter import for sample status
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/test.xlsx
+++ b/baobab/lims/setupdata/test/test.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="1115">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -2487,6 +2487,9 @@
     <t xml:space="preserve">Def 002</t>
   </si>
   <si>
+    <t xml:space="preserve">Receive</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 3</t>
   </si>
   <si>
@@ -2533,6 +2536,36 @@
   </si>
   <si>
     <t xml:space="preserve">Def 006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gobbledygook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Sample 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test sample 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Def 007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Sample 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test sample 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Def 008</t>
   </si>
   <si>
     <t xml:space="preserve">Register</t>
@@ -3470,7 +3503,7 @@
     <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="171" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3709,13 +3742,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3796,7 +3822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="180">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4447,10 +4473,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -4606,7 +4628,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="110.866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="111.834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="6.85425101214575"/>
   </cols>
   <sheetData>
@@ -4676,7 +4698,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.3886639676113"/>
@@ -4994,9 +5016,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="21" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -5271,11 +5293,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -5448,9 +5470,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5518,7 +5540,7 @@
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5663,12 +5685,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
@@ -5936,11 +5958,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6041,9 +6063,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6134,11 +6156,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -6647,10 +6669,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -6720,12 +6742,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
@@ -7076,8 +7098,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7127,8 +7149,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7181,7 +7203,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -7301,7 +7323,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
@@ -7472,9 +7494,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -7551,7 +7573,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -7930,11 +7952,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.0242914979757"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
@@ -8170,10 +8192,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="64.7004048582996"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="65.2348178137652"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="96" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8347,8 +8369,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -8419,26 +8441,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8708,8 +8730,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -9103,18 +9125,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="44.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9265,17 +9287,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9418,9 +9440,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -9521,14 +9543,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -9699,12 +9721,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="6.42914979757085"/>
   </cols>
   <sheetData>
@@ -9837,26 +9859,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5991902834008"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9"/>
     <col collapsed="false" hidden="false" max="13" min="9" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9971,7 +9994,7 @@
       <c r="O3" s="6" t="s">
         <v>769</v>
       </c>
-      <c r="P3" s="163" t="s">
+      <c r="P3" s="6" t="s">
         <v>770</v>
       </c>
     </row>
@@ -10044,15 +10067,15 @@
       </c>
       <c r="O5" s="40"/>
       <c r="P5" s="0" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C6" s="79" t="s">
         <v>433</v>
@@ -10062,11 +10085,11 @@
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="88" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="G6" s="89"/>
       <c r="H6" s="89" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>30</v>
@@ -10080,15 +10103,15 @@
       </c>
       <c r="O6" s="40"/>
       <c r="P6" s="0" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C7" s="79" t="s">
         <v>433</v>
@@ -10098,7 +10121,7 @@
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="88" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="G7" s="89"/>
       <c r="H7" s="89"/>
@@ -10116,10 +10139,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>433</v>
@@ -10129,11 +10152,11 @@
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="88" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="G8" s="89"/>
       <c r="H8" s="89" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I8" s="5" t="n">
         <v>15</v>
@@ -10149,10 +10172,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C9" s="79" t="s">
         <v>433</v>
@@ -10162,11 +10185,11 @@
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="88" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="G9" s="89"/>
       <c r="H9" s="89" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>10</v>
@@ -10180,7 +10203,79 @@
       </c>
       <c r="O9" s="40"/>
       <c r="P9" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>799</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>800</v>
+      </c>
+      <c r="C10" s="79" t="s">
+        <v>433</v>
+      </c>
+      <c r="D10" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="79"/>
+      <c r="F10" s="88" t="s">
+        <v>801</v>
+      </c>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89" t="s">
+        <v>802</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="L10" s="93"/>
+      <c r="N10" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="O10" s="40"/>
+      <c r="P10" s="0" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>805</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>433</v>
+      </c>
+      <c r="D11" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="79"/>
+      <c r="F11" s="88" t="s">
+        <v>806</v>
+      </c>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89" t="s">
+        <v>807</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="L11" s="93"/>
+      <c r="N11" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="O11" s="40"/>
+      <c r="P11" s="0" t="s">
+        <v>808</v>
       </c>
     </row>
   </sheetData>
@@ -10208,10 +10303,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -10223,15 +10318,15 @@
       <c r="B1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="164" t="s">
+      <c r="C1" s="163" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="14" t="s">
-        <v>798</v>
-      </c>
-      <c r="C2" s="165"/>
+        <v>809</v>
+      </c>
+      <c r="C2" s="164"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
@@ -10240,73 +10335,73 @@
       <c r="B3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="163" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>799</v>
+        <v>810</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>800</v>
-      </c>
-      <c r="C4" s="166" t="n">
+        <v>811</v>
+      </c>
+      <c r="C4" s="165" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>801</v>
+        <v>812</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>802</v>
-      </c>
-      <c r="C5" s="166" t="n">
+        <v>813</v>
+      </c>
+      <c r="C5" s="165" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>803</v>
+        <v>814</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>803</v>
-      </c>
-      <c r="C6" s="166" t="s">
-        <v>804</v>
+        <v>814</v>
+      </c>
+      <c r="C6" s="165" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>805</v>
+        <v>816</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>806</v>
-      </c>
-      <c r="C7" s="167" t="n">
+        <v>817</v>
+      </c>
+      <c r="C7" s="166" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>807</v>
+        <v>818</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>808</v>
-      </c>
-      <c r="C8" s="167" t="n">
+        <v>819</v>
+      </c>
+      <c r="C8" s="166" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>809</v>
+        <v>820</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>810</v>
-      </c>
-      <c r="C9" s="166" t="n">
+        <v>821</v>
+      </c>
+      <c r="C9" s="165" t="n">
         <v>15</v>
       </c>
     </row>
@@ -10315,240 +10410,240 @@
         <v>498</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>811</v>
-      </c>
-      <c r="C10" s="166" t="n">
+        <v>822</v>
+      </c>
+      <c r="C10" s="165" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>812</v>
+        <v>823</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>813</v>
-      </c>
-      <c r="C11" s="166" t="n">
+        <v>824</v>
+      </c>
+      <c r="C11" s="165" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>815</v>
-      </c>
-      <c r="C12" s="166" t="n">
+        <v>826</v>
+      </c>
+      <c r="C12" s="165" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>816</v>
+        <v>827</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>817</v>
-      </c>
-      <c r="C13" s="166" t="n">
+        <v>828</v>
+      </c>
+      <c r="C13" s="165" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>818</v>
+        <v>829</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>819</v>
-      </c>
-      <c r="C14" s="166"/>
+        <v>830</v>
+      </c>
+      <c r="C14" s="165"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>820</v>
+        <v>831</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>821</v>
-      </c>
-      <c r="C15" s="167" t="n">
+        <v>832</v>
+      </c>
+      <c r="C15" s="166" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>822</v>
+        <v>833</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>823</v>
-      </c>
-      <c r="C16" s="167" t="n">
+        <v>834</v>
+      </c>
+      <c r="C16" s="166" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>824</v>
+        <v>835</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>825</v>
-      </c>
-      <c r="C17" s="167" t="n">
+        <v>836</v>
+      </c>
+      <c r="C17" s="166" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>826</v>
+        <v>837</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>827</v>
-      </c>
-      <c r="C18" s="168" t="s">
-        <v>828</v>
-      </c>
-      <c r="D18" s="169"/>
+        <v>838</v>
+      </c>
+      <c r="C18" s="167" t="s">
+        <v>839</v>
+      </c>
+      <c r="D18" s="168"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>829</v>
+        <v>840</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>830</v>
-      </c>
-      <c r="C19" s="170" t="s">
+        <v>841</v>
+      </c>
+      <c r="C19" s="169" t="s">
         <v>301</v>
       </c>
-      <c r="D19" s="169"/>
+      <c r="D19" s="168"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>831</v>
+        <v>842</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>832</v>
-      </c>
-      <c r="C20" s="170" t="s">
+        <v>843</v>
+      </c>
+      <c r="C20" s="169" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>833</v>
+        <v>844</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>834</v>
-      </c>
-      <c r="C21" s="168" t="n">
+        <v>845</v>
+      </c>
+      <c r="C21" s="167" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>835</v>
+        <v>846</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>836</v>
-      </c>
-      <c r="C22" s="168" t="n">
+        <v>847</v>
+      </c>
+      <c r="C22" s="167" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>837</v>
+        <v>848</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>838</v>
-      </c>
-      <c r="C23" s="168" t="n">
+        <v>849</v>
+      </c>
+      <c r="C23" s="167" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>839</v>
+        <v>850</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>840</v>
-      </c>
-      <c r="C24" s="170" t="s">
-        <v>841</v>
-      </c>
-      <c r="D24" s="171"/>
+        <v>851</v>
+      </c>
+      <c r="C24" s="169" t="s">
+        <v>852</v>
+      </c>
+      <c r="D24" s="170"/>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>842</v>
+        <v>853</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>843</v>
-      </c>
-      <c r="C25" s="170" t="s">
-        <v>844</v>
+        <v>854</v>
+      </c>
+      <c r="C25" s="169" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>845</v>
+        <v>856</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>846</v>
-      </c>
-      <c r="C26" s="167" t="n">
+        <v>857</v>
+      </c>
+      <c r="C26" s="166" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>847</v>
+        <v>858</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>848</v>
-      </c>
-      <c r="C27" s="166" t="s">
+        <v>859</v>
+      </c>
+      <c r="C27" s="165" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>849</v>
+        <v>860</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>850</v>
-      </c>
-      <c r="C28" s="166" t="n">
+        <v>861</v>
+      </c>
+      <c r="C28" s="165" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>851</v>
+        <v>862</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>852</v>
-      </c>
-      <c r="C29" s="167" t="n">
+        <v>863</v>
+      </c>
+      <c r="C29" s="166" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>853</v>
+        <v>864</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>854</v>
-      </c>
-      <c r="C30" s="166"/>
+        <v>865</v>
+      </c>
+      <c r="C30" s="165"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>855</v>
+        <v>866</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>856</v>
-      </c>
-      <c r="C31" s="172" t="s">
-        <v>857</v>
+        <v>867</v>
+      </c>
+      <c r="C31" s="171" t="s">
+        <v>868</v>
       </c>
     </row>
   </sheetData>
@@ -10687,35 +10782,35 @@
   </cols>
   <sheetData>
     <row r="1" s="31" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="172" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="173" t="s">
+      <c r="B1" s="172" t="s">
         <v>198</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>858</v>
+        <v>869</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>859</v>
+        <v>870</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>860</v>
+        <v>871</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>861</v>
-      </c>
-      <c r="G1" s="174" t="s">
-        <v>862</v>
+        <v>872</v>
+      </c>
+      <c r="G1" s="173" t="s">
+        <v>873</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>863</v>
+        <v>874</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>864</v>
+        <v>875</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>865</v>
+        <v>876</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>511</v>
@@ -10730,63 +10825,63 @@
         <v>243</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>828</v>
+        <v>839</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>866</v>
-      </c>
-      <c r="E2" s="175" t="s">
-        <v>867</v>
+        <v>877</v>
+      </c>
+      <c r="E2" s="174" t="s">
+        <v>878</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>868</v>
+        <v>879</v>
       </c>
       <c r="G2" s="51" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>869</v>
+        <v>880</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>870</v>
+        <v>881</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>871</v>
+        <v>882</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>872</v>
+        <v>883</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>873</v>
+        <v>884</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>874</v>
+        <v>885</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>301</v>
       </c>
-      <c r="E3" s="175" t="s">
-        <v>844</v>
+      <c r="E3" s="174" t="s">
+        <v>855</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>875</v>
+        <v>886</v>
       </c>
       <c r="G3" s="51" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="51" t="s">
-        <v>876</v>
+        <v>887</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>877</v>
+        <v>888</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>878</v>
+        <v>889</v>
       </c>
       <c r="K3" s="51" t="s">
         <v>535</v>
@@ -10794,51 +10889,51 @@
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>879</v>
+        <v>890</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>225</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>880</v>
+        <v>891</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>881</v>
+        <v>892</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>841</v>
-      </c>
-      <c r="G4" s="175"/>
+        <v>852</v>
+      </c>
+      <c r="G4" s="174"/>
       <c r="H4" s="51" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>882</v>
+        <v>893</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>883</v>
-      </c>
-      <c r="G5" s="175"/>
+        <v>894</v>
+      </c>
+      <c r="G5" s="174"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>884</v>
+        <v>895</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>885</v>
-      </c>
-      <c r="G6" s="175"/>
+        <v>896</v>
+      </c>
+      <c r="G6" s="174"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>886</v>
+        <v>897</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>887</v>
-      </c>
-      <c r="G7" s="175"/>
+        <v>898</v>
+      </c>
+      <c r="G7" s="174"/>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
@@ -10847,108 +10942,108 @@
       <c r="B8" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="G8" s="175"/>
+      <c r="G8" s="174"/>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="175"/>
+      <c r="G9" s="174"/>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="175"/>
+      <c r="G10" s="174"/>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="175"/>
+      <c r="G11" s="174"/>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="175"/>
+      <c r="G12" s="174"/>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="175"/>
+      <c r="G13" s="174"/>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="175"/>
+      <c r="G14" s="174"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="175"/>
+      <c r="G15" s="174"/>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="175"/>
+      <c r="G16" s="174"/>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="175"/>
+      <c r="G17" s="174"/>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="175"/>
+      <c r="G18" s="174"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="175"/>
+      <c r="G19" s="174"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="176"/>
-      <c r="B20" s="176"/>
-      <c r="C20" s="176"/>
-      <c r="D20" s="176"/>
-      <c r="E20" s="177"/>
-      <c r="F20" s="176"/>
-      <c r="G20" s="177"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176"/>
-      <c r="J20" s="176"/>
-      <c r="K20" s="176"/>
-      <c r="L20" s="176"/>
-    </row>
-    <row r="21" s="179" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="175"/>
+      <c r="B20" s="175"/>
+      <c r="C20" s="175"/>
+      <c r="D20" s="175"/>
+      <c r="E20" s="176"/>
+      <c r="F20" s="175"/>
+      <c r="G20" s="176"/>
+      <c r="H20" s="175"/>
+      <c r="I20" s="175"/>
+      <c r="J20" s="175"/>
+      <c r="K20" s="175"/>
+      <c r="L20" s="175"/>
+    </row>
+    <row r="21" s="178" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>888</v>
+        <v>899</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>803</v>
+        <v>814</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>889</v>
+        <v>900</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>890</v>
-      </c>
-      <c r="E21" s="178" t="s">
-        <v>891</v>
+        <v>901</v>
+      </c>
+      <c r="E21" s="177" t="s">
+        <v>902</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>892</v>
+        <v>903</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>893</v>
+        <v>904</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>894</v>
+        <v>905</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>895</v>
+        <v>906</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="180" t="s">
-        <v>896</v>
+      <c r="A22" s="179" t="s">
+        <v>907</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>897</v>
+        <v>908</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>898</v>
+        <v>909</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>899</v>
-      </c>
-      <c r="E22" s="175" t="s">
-        <v>900</v>
+        <v>910</v>
+      </c>
+      <c r="E22" s="174" t="s">
+        <v>911</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>901</v>
+        <v>912</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>902</v>
+        <v>913</v>
       </c>
       <c r="H22" s="51" t="s">
-        <v>902</v>
+        <v>913</v>
       </c>
       <c r="I22" s="51" t="s">
         <v>520</v>
@@ -10956,970 +11051,970 @@
     </row>
     <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="51" t="s">
-        <v>903</v>
+        <v>914</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>904</v>
+        <v>915</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>905</v>
-      </c>
-      <c r="E23" s="175" t="s">
-        <v>906</v>
+        <v>916</v>
+      </c>
+      <c r="E23" s="174" t="s">
+        <v>917</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>907</v>
+        <v>918</v>
       </c>
       <c r="G23" s="51" t="s">
-        <v>908</v>
+        <v>919</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>908</v>
+        <v>919</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>909</v>
+        <v>920</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="51" t="s">
-        <v>910</v>
+        <v>921</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>911</v>
+        <v>922</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>912</v>
+        <v>923</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>913</v>
+        <v>924</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>914</v>
+        <v>925</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>914</v>
+        <v>925</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>915</v>
+        <v>926</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="51" t="s">
-        <v>916</v>
+        <v>927</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>918</v>
+        <v>929</v>
       </c>
       <c r="H25" s="51" t="s">
-        <v>919</v>
+        <v>930</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>920</v>
+        <v>931</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="51" t="s">
-        <v>921</v>
+        <v>932</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>922</v>
+        <v>933</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>923</v>
+        <v>934</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="51" t="s">
-        <v>924</v>
+        <v>935</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>925</v>
+        <v>936</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="51" t="s">
-        <v>926</v>
+        <v>937</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>927</v>
+        <v>938</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="51" t="s">
-        <v>928</v>
+        <v>939</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>929</v>
+        <v>940</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="51" t="s">
-        <v>930</v>
+        <v>941</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>931</v>
+        <v>942</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="51" t="s">
-        <v>932</v>
+        <v>943</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>933</v>
+        <v>944</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="51" t="s">
-        <v>934</v>
+        <v>945</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>935</v>
+        <v>946</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="51" t="s">
-        <v>936</v>
+        <v>947</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>937</v>
+        <v>948</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="51" t="s">
-        <v>938</v>
+        <v>949</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="51" t="s">
-        <v>939</v>
+        <v>950</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="51" t="s">
-        <v>940</v>
+        <v>951</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="51" t="s">
-        <v>941</v>
+        <v>952</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="51" t="s">
-        <v>942</v>
+        <v>953</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="51" t="s">
-        <v>943</v>
+        <v>954</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="51" t="s">
-        <v>944</v>
+        <v>955</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="51" t="s">
-        <v>945</v>
+        <v>956</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="51" t="s">
-        <v>946</v>
+        <v>957</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="51" t="s">
-        <v>947</v>
+        <v>958</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="51" t="s">
-        <v>948</v>
+        <v>959</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="51" t="s">
-        <v>949</v>
+        <v>960</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="51" t="s">
-        <v>950</v>
+        <v>961</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="51" t="s">
-        <v>951</v>
+        <v>962</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="51" t="s">
-        <v>952</v>
+        <v>963</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="51" t="s">
-        <v>953</v>
+        <v>964</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="51" t="s">
-        <v>954</v>
+        <v>965</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="51" t="s">
-        <v>955</v>
+        <v>966</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="51" t="s">
-        <v>956</v>
+        <v>967</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="51" t="s">
-        <v>957</v>
+        <v>968</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="51" t="s">
-        <v>958</v>
+        <v>969</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="51" t="s">
-        <v>959</v>
+        <v>970</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="51" t="s">
-        <v>960</v>
+        <v>971</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="51" t="s">
-        <v>961</v>
+        <v>972</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="51" t="s">
-        <v>962</v>
+        <v>973</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="51" t="s">
-        <v>963</v>
+        <v>974</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="51" t="s">
-        <v>964</v>
+        <v>975</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="51" t="s">
-        <v>965</v>
+        <v>976</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="51" t="s">
-        <v>966</v>
+        <v>977</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="51" t="s">
-        <v>967</v>
+        <v>978</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="51" t="s">
-        <v>968</v>
+        <v>979</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="51" t="s">
-        <v>969</v>
+        <v>980</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="51" t="s">
-        <v>970</v>
+        <v>981</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="51" t="s">
-        <v>971</v>
+        <v>982</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="51" t="s">
-        <v>972</v>
+        <v>983</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="51" t="s">
-        <v>973</v>
+        <v>984</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="51" t="s">
-        <v>974</v>
+        <v>985</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="51" t="s">
-        <v>975</v>
+        <v>986</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="51" t="s">
-        <v>976</v>
+        <v>987</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="51" t="s">
-        <v>977</v>
+        <v>988</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="51" t="s">
-        <v>978</v>
+        <v>989</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="51" t="s">
-        <v>979</v>
+        <v>990</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="51" t="s">
-        <v>980</v>
+        <v>991</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="51" t="s">
-        <v>981</v>
+        <v>992</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="51" t="s">
-        <v>982</v>
+        <v>993</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="51" t="s">
-        <v>983</v>
+        <v>994</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="51" t="s">
-        <v>984</v>
+        <v>995</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="51" t="s">
-        <v>985</v>
+        <v>996</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="51" t="s">
-        <v>986</v>
+        <v>997</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="51" t="s">
-        <v>987</v>
+        <v>998</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="51" t="s">
-        <v>988</v>
+        <v>999</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="51" t="s">
-        <v>989</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="51" t="s">
-        <v>990</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="51" t="s">
-        <v>991</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="51" t="s">
-        <v>992</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="51" t="s">
-        <v>993</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="51" t="s">
-        <v>994</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="51" t="s">
-        <v>995</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="51" t="s">
-        <v>996</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="51" t="s">
-        <v>997</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="51" t="s">
-        <v>998</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="51" t="s">
-        <v>999</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="51" t="s">
-        <v>1000</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="51" t="s">
-        <v>1001</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="51" t="s">
-        <v>1002</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="51" t="s">
-        <v>1003</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="51" t="s">
-        <v>1004</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="51" t="s">
-        <v>1005</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="51" t="s">
-        <v>1006</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="51" t="s">
-        <v>1007</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="51" t="s">
-        <v>1008</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="51" t="s">
-        <v>1009</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="51" t="s">
-        <v>1010</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="51" t="s">
-        <v>1011</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="51" t="s">
-        <v>1012</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="51" t="s">
-        <v>1013</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="51" t="s">
-        <v>1014</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="51" t="s">
-        <v>1015</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="51" t="s">
-        <v>1016</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="51" t="s">
-        <v>1017</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="51" t="s">
-        <v>1018</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="51" t="s">
-        <v>1019</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="51" t="s">
-        <v>1020</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="51" t="s">
-        <v>1021</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="51" t="s">
-        <v>1022</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="51" t="s">
-        <v>1023</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="51" t="s">
-        <v>1024</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="51" t="s">
-        <v>1025</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="51" t="s">
-        <v>1026</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="51" t="s">
-        <v>1027</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="51" t="s">
-        <v>1028</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="51" t="s">
-        <v>1029</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="51" t="s">
-        <v>1030</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="51" t="s">
-        <v>1031</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="51" t="s">
-        <v>1032</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="51" t="s">
-        <v>1033</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="51" t="s">
-        <v>1034</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="51" t="s">
-        <v>1035</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="51" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="51" t="s">
-        <v>1037</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="51" t="s">
-        <v>1038</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="51" t="s">
-        <v>1039</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="51" t="s">
-        <v>1040</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="51" t="s">
-        <v>1041</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="51" t="s">
-        <v>1042</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="51" t="s">
-        <v>1043</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="51" t="s">
-        <v>1044</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="51" t="s">
-        <v>1045</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="51" t="s">
-        <v>1046</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="51" t="s">
-        <v>1047</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="51" t="s">
-        <v>1048</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="51" t="s">
-        <v>1049</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="51" t="s">
-        <v>1050</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="51" t="s">
-        <v>1051</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="51" t="s">
-        <v>1052</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="51" t="s">
-        <v>1053</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="51" t="s">
-        <v>1054</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="51" t="s">
-        <v>1055</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="51" t="s">
-        <v>1056</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="51" t="s">
-        <v>1057</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="51" t="s">
-        <v>1058</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="51" t="s">
-        <v>1059</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="51" t="s">
-        <v>1060</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="51" t="s">
-        <v>1061</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="51" t="s">
-        <v>1062</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="51" t="s">
-        <v>1063</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="51" t="s">
-        <v>1064</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="51" t="s">
-        <v>1065</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="51" t="s">
-        <v>1066</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="51" t="s">
-        <v>1067</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="51" t="s">
-        <v>1068</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="51" t="s">
-        <v>1069</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="51" t="s">
-        <v>1070</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="51" t="s">
-        <v>1071</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="51" t="s">
-        <v>1072</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="51" t="s">
-        <v>1073</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="51" t="s">
-        <v>1074</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="51" t="s">
-        <v>1075</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="51" t="s">
-        <v>1076</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="51" t="s">
-        <v>1077</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="51" t="s">
-        <v>1078</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="51" t="s">
-        <v>1079</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="51" t="s">
-        <v>1080</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="51" t="s">
-        <v>1081</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="51" t="s">
-        <v>1082</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="51" t="s">
-        <v>1083</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="51" t="s">
-        <v>1084</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="51" t="s">
-        <v>1085</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="51" t="s">
-        <v>1086</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="51" t="s">
-        <v>1087</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="51" t="s">
-        <v>1088</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="51" t="s">
-        <v>1089</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="51" t="s">
-        <v>1090</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="51" t="s">
-        <v>1091</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="51" t="s">
-        <v>1092</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="51" t="s">
-        <v>1093</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="51" t="s">
-        <v>1094</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="51" t="s">
-        <v>1095</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="51" t="s">
-        <v>1096</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="51" t="s">
-        <v>1097</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="51" t="s">
-        <v>1098</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="51" t="s">
-        <v>1099</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="51" t="s">
-        <v>1100</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="51" t="s">
-        <v>1101</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="51" t="s">
-        <v>804</v>
+        <v>815</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="51" t="s">
-        <v>1102</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="51" t="s">
-        <v>1103</v>
+        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -11950,8 +12045,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="28" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -12123,7 +12218,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74898785425101"/>
@@ -12328,7 +12423,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
@@ -12487,7 +12582,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
@@ -12496,7 +12591,7 @@
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -12966,13 +13061,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
@@ -13335,9 +13430,9 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
Work saving check in
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/test.xlsx
+++ b/baobab/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="34"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -69,7 +69,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">From the manual: 'Some Analyses requiring text input as results is best limited to a number of known possible outcomes to prevent typos and irrelevant input skewing reporting. 
 The known outcomes, e.g. 'Positive' or 'Negative',  can be pre-configured here and only these allowed when results are captured. These will be offered as options on a drop-down menu on the data capturing screens'</t>
@@ -93,7 +92,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The sample type abbreviation must be unique – it is used as prefix to sample records</t>
         </r>
@@ -117,7 +115,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Only if a Client Contact is a LIMS user too, does he/she get given a (unique) user name and password</t>
         </r>
@@ -131,7 +128,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Please copy from other contacts for the same Client on this sheet: Use contact Fullname (Firstname + “ “ + Lastname). If more than one needs to be cc'd, please separate with commas. Only contacts for the same client are valid.</t>
         </r>
@@ -142,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="1115">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -2445,12 +2441,18 @@
     <t xml:space="preserve">SampleType</t>
   </si>
   <si>
+    <t xml:space="preserve">SampleState</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biospecimens</t>
   </si>
   <si>
     <t xml:space="preserve">Linked Sample</t>
   </si>
   <si>
+    <t xml:space="preserve">Sample State: register, due or received(default)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 1</t>
   </si>
   <si>
@@ -2466,6 +2468,9 @@
     <t xml:space="preserve">ml</t>
   </si>
   <si>
+    <t xml:space="preserve">due</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 2</t>
   </si>
   <si>
@@ -2478,6 +2483,9 @@
     <t xml:space="preserve">Def 002</t>
   </si>
   <si>
+    <t xml:space="preserve">Receive</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 3</t>
   </si>
   <si>
@@ -2490,6 +2498,9 @@
     <t xml:space="preserve">Def 003</t>
   </si>
   <si>
+    <t xml:space="preserve">Due</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 4</t>
   </si>
   <si>
@@ -2523,49 +2534,37 @@
     <t xml:space="preserve">Def 006</t>
   </si>
   <si>
+    <t xml:space="preserve">gobbledygook</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 7</t>
   </si>
   <si>
     <t xml:space="preserve">Test sample 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Room-2.Freezer-1.Box-01.15</t>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.17</t>
   </si>
   <si>
     <t xml:space="preserve">Def 007</t>
   </si>
   <si>
+    <t xml:space="preserve">received</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 8</t>
   </si>
   <si>
     <t xml:space="preserve">Test sample 8</t>
   </si>
   <si>
-    <t xml:space="preserve">Room-2.Freezer-1.Box-01.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Sample 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test sample 9</t>
-  </si>
-  <si>
     <t xml:space="preserve">Room-2.Freezer-1.Box-01.18</t>
   </si>
   <si>
-    <t xml:space="preserve">Def 009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Sample 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test sample 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room-2.Freezer-1.Box-01.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Def 010</t>
+    <t xml:space="preserve">Def 008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
   </si>
   <si>
     <t xml:space="preserve">Setup – Global defaults</t>
@@ -3506,7 +3505,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3529,21 +3527,18 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3551,20 +3546,17 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3572,7 +3564,6 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3580,14 +3571,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3595,14 +3584,12 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3610,27 +3597,23 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="FreeSans"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="FreeSans"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3638,41 +3621,35 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="FreeSans"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="FreeSans"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3680,7 +3657,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3688,7 +3664,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3696,7 +3671,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3705,7 +3679,6 @@
       <color rgb="FF2323DC"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3713,7 +3686,6 @@
       <color rgb="FF000000"/>
       <name val="Arla"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3721,7 +3693,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3729,7 +3700,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3737,7 +3707,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4625,7 +4594,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="106.153846153846"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="112.797570850202"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="6.85425101214575"/>
   </cols>
   <sheetData>
@@ -4695,7 +4664,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.3886639676113"/>
@@ -4982,7 +4951,7 @@
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="true" error="Only ISO 3166 countries are valid" errorTitle="Please select a valid country from the drop-down" operator="equal" prompt="Valid ISO 3166 countries for selection" promptTitle="Select a country from the drop down lits" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J4:J5 O4:O5 T4:T5" type="list">
-      <formula1>#ref!!#ref!</formula1>
+      <formula1>#REF! #REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5013,9 +4982,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="10" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="21" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -5290,11 +5259,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -5467,9 +5436,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5537,7 +5506,7 @@
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5682,12 +5651,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
@@ -5955,11 +5924,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6060,9 +6029,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6153,11 +6122,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -6578,56 +6547,8 @@
     <mergeCell ref="P2:R2"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q4:Q5" type="whole">
-      <formula1>0</formula1>
-      <formula2>23</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R4:R5" type="whole">
-      <formula1>0</formula1>
-      <formula2>59</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" prompt="The unique keyword used to identify the analysis service in import files of bulk AR requests and results imports from instruments. It is also used to identify dependent analysis services in user defined results calculations" promptTitle="Unique Analysis Service keyword" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="D4:D5" type="none">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select 1 or 0 from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (true)  or 0 (false) from the drop-down menu" promptTitle="Can the result be expressed as % dry matter?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H5" type="list">
-      <formula1>#ref!!$G$2:$G$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Indicates whether file attachments are required, permitted  or not for the analysis service" promptTitle="Analysis attachment option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I4:I5" type="list">
-      <formula1>#ref!!$D$2:$D$20</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number greater than or equal to 0" errorTitle="Invalid data" operator="greaterThanOrEqual" prompt="Please enter a whole number greater than or equal to 0" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P4:P5" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid method from the selection list" errorTitle="Invalid method" operator="equal" prompt="Select a method from the selection list. Maintain the list of valid options on the 'Methods' sheet" promptTitle="Select a valid Method" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W4:W5" type="list">
-      <formula1>#ref!!$A$4:$A$84</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select an instrument from the selection list. Maintain the list of valid options on the 'Instruments' sheet" promptTitle="Select a valid Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X4:X5" type="list">
-      <formula1>#ref!!$A$4:$A$43</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select a Calculation from the selection list. Maintain the list of valid options on the 'Calculations' sheet" promptTitle="Select a valid Calculation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y4:Y5" type="list">
-      <formula1>#ref!!$A$4:$A$97</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select 1  or 0 from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (true) or 0 (false) from the drop-down menu" promptTitle="Is the analysis accredited?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AA4:AA5" type="list">
-      <formula1>#ref!!$G$2:$G$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select 1 or 0 from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (true) or 0 (false) from the drop-down menu" promptTitle="Does this analysis require a separate sample partition?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB4:AB5" type="list">
-      <formula1>#ref!!$G$2:$G$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select a Container from the selection list. Maintain the list of valid options on the 'Containers' sheet." promptTitle="Select a valid Container" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC4:AC5" type="list">
-      <formula1>'AnalysisService ResultOptions'!$A$4:$A$242</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select a Preservation from the selection list. Maintain the list of valid options on the 'Preservations' sheet." promptTitle="Select a valid Preservation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD4:AD5" type="list">
-      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select a valid entry from the drop-down menu" promptTitle="Field or Lab analysis?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E5" type="list">
@@ -6640,6 +6561,54 @@
     </dataValidation>
     <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid entry from the drop-down menu" promptTitle="Valid data entry" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G5" type="list">
       <formula1>'Lab Departments'!$A$4:$A$52</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select 1 or 0 from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (true)  or 0 (false) from the drop-down menu" promptTitle="Can the result be expressed as % dry matter?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H5" type="list">
+      <formula1>#REF! $G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Indicates whether file attachments are required, permitted  or not for the analysis service" promptTitle="Analysis attachment option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I4:I5" type="list">
+      <formula1>#REF! $D$2:$D$20</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please enter a whole number greater than or equal to 0" errorTitle="Invalid data" operator="greaterThanOrEqual" prompt="Please enter a whole number greater than or equal to 0" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P4:P5" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q4:Q5" type="whole">
+      <formula1>0</formula1>
+      <formula2>23</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R4:R5" type="whole">
+      <formula1>0</formula1>
+      <formula2>59</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Select a valid method from the selection list" errorTitle="Invalid method" operator="equal" prompt="Select a method from the selection list. Maintain the list of valid options on the 'Methods' sheet" promptTitle="Select a valid Method" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W4:W5" type="list">
+      <formula1>#REF! $A$4:$A$84</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select an instrument from the selection list. Maintain the list of valid options on the 'Instruments' sheet" promptTitle="Select a valid Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X4:X5" type="list">
+      <formula1>#REF! $A$4:$A$43</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select a Calculation from the selection list. Maintain the list of valid options on the 'Calculations' sheet" promptTitle="Select a valid Calculation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y4:Y5" type="list">
+      <formula1>#REF! $A$4:$A$97</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select 1  or 0 from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (true) or 0 (false) from the drop-down menu" promptTitle="Is the analysis accredited?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AA4:AA5" type="list">
+      <formula1>#REF! $G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select 1 or 0 from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (true) or 0 (false) from the drop-down menu" promptTitle="Does this analysis require a separate sample partition?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB4:AB5" type="list">
+      <formula1>#REF! $G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select a Container from the selection list. Maintain the list of valid options on the 'Containers' sheet." promptTitle="Select a valid Container" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC4:AC5" type="list">
+      <formula1>'AnalysisService ResultOptions'!$A$4:$A$242</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Select a valid instrument from the selection list" errorTitle="Invalid Instrument" operator="equal" prompt="Select a Preservation from the selection list. Maintain the list of valid options on the 'Preservations' sheet." promptTitle="Select a valid Preservation" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD4:AD5" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -6666,10 +6635,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -6739,12 +6708,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
@@ -7095,8 +7064,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7146,8 +7115,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7200,7 +7169,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -7281,11 +7250,11 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Analysis Service" operator="equal" prompt="Select an Analysis Service  from the list. Maintain the list on the 'Analysis Services' sheet" promptTitle="Select an Analysis Service" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A1:C2 A3 C3" type="list">
-      <formula1>#ref!!$A$4:$A$141</formula1>
+      <formula1>#REF! $A$4:$A$141</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Analysis Service" operator="equal" prompt="Select an Analysis Service  from the list. Maintain the list on the 'Analysis Services' sheet" promptTitle="Select an Analysis Service" showDropDown="true" showErrorMessage="false" showInputMessage="false" sqref="B3" type="list">
-      <formula1>#ref!!$A$4:$A$141</formula1>
+      <formula1>#REF! $A$4:$A$141</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Analysis Service" operator="equal" prompt="Select an Analysis Service  from the list. Maintain the list on the 'Analysis Services' sheet" promptTitle="Select an Analysis Service" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A6" type="list">
@@ -7320,7 +7289,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
@@ -7491,9 +7460,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -7570,7 +7539,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -7914,12 +7883,12 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A6:A85" type="list">
-      <formula1>#ref!!$A$4:$A$52</formula1>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4:A5" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4:A5" type="list">
-      <formula1>#ref!</formula1>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A6:A85" type="list">
+      <formula1>#REF! $A$4:$A$52</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -7943,16 +7912,18 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8026,7 +7997,7 @@
         <v>596</v>
       </c>
       <c r="C4" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D4" s="89" t="s">
         <v>597</v>
@@ -8050,7 +8021,7 @@
         <v>601</v>
       </c>
       <c r="C5" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D5" s="89" t="s">
         <v>602</v>
@@ -8074,7 +8045,7 @@
         <v>606</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D6" s="89" t="s">
         <v>607</v>
@@ -8098,7 +8069,7 @@
         <v>611</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D7" s="89" t="s">
         <v>612</v>
@@ -8122,7 +8093,7 @@
         <v>616</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D8" s="89" t="s">
         <v>617</v>
@@ -8146,7 +8117,7 @@
         <v>621</v>
       </c>
       <c r="C9" s="88" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D9" s="89" t="s">
         <v>622</v>
@@ -8187,10 +8158,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="61.914979757085"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="65.7692307692308"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="96" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8329,12 +8300,12 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4" type="list">
-      <formula1>#ref!!$A$4:$A$500</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4" type="list">
+      <formula1>Calculations!$A$4:$A$500</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4" type="list">
-      <formula1>Calculations!$A$4:$A$500</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4" type="list">
+      <formula1>#REF! $A$4:$A$500</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -8364,8 +8335,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -8436,26 +8407,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8689,11 +8660,11 @@
       <formula1>'Instrument Types'!$A$4:$A$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Instrument Type" operator="equal" prompt="Select an Instrument Type  from the list. Maintain the list on the 'Instrument Types' sheet" promptTitle="Select an Instrument Type" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4" type="list">
+    <dataValidation allowBlank="true" error="Select a valid entry from the drop down list." errorTitle="Invalid Manufacturer" operator="equal" prompt="Select a Manufacturer from the list. Maintain the list on the 'Manufacturers' sheet" promptTitle="Select a Manufacturer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="list">
       <formula1>Suppliers!$A$4:$A$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid entry from the drop down list." errorTitle="Invalid Manufacturer" operator="equal" prompt="Select a Manufacturer from the list. Maintain the list on the 'Manufacturers' sheet" promptTitle="Select a Manufacturer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="list">
+    <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Instrument Type" operator="equal" prompt="Select an Instrument Type  from the list. Maintain the list on the 'Instrument Types' sheet" promptTitle="Select an Instrument Type" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4" type="list">
       <formula1>Suppliers!$A$4:$A$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8725,8 +8696,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -9080,15 +9051,15 @@
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation allowBlank="false" error="Select TRUE or FALSE from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select TRUE or FALSE from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E5 D11" type="list">
+      <formula1>$#REF!.$G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" errorTitle="Invalid entry" operator="between" prompt="Between 0 and 100" promptTitle="Enter a % value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6 D10" type="decimal">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C7" type="list">
-      <formula1>$#REF!.$G$2:$G$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select TRUE or FALSE from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select TRUE or FALSE from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E5 D11" type="list">
       <formula1>$#REF!.$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9120,18 +9091,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="44.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9250,12 +9221,12 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation allowBlank="true" error="Select a valid instrument from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Instruments' sheet" promptTitle="Select an Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
+      <formula1>Instruments!$B$4:$B$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" error="Not a date" errorTitle="Invalid entry" operator="greaterThan" prompt="After 1 Jan 2012. Expected format is YYYY/MM/DD" promptTitle="Please enter a date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:E4" type="date">
       <formula1>40909</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Instruments' sheet" promptTitle="Select an Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
-      <formula1>Instruments!$B$4:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -9282,17 +9253,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9401,12 +9372,12 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation allowBlank="true" error="Select a valid instrument from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Instruments' sheet" promptTitle="Select an Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
+      <formula1>Instruments!$B$4:$B$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" error="Not a date" errorTitle="Invalid entry" operator="greaterThan" prompt="After 1 Jan 2012. Expected format is YYYY/MM/DD" promptTitle="Please enter a date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:E4" type="date">
       <formula1>40909</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Instruments' sheet" promptTitle="Select an Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
-      <formula1>Instruments!$B$4:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -9435,9 +9406,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -9537,15 +9508,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.3846153846154"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -9683,12 +9654,12 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation allowBlank="true" error="Select a valid instrument from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Instruments' sheet" promptTitle="Select an Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
+      <formula1>Instruments!$B$4:$B$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" error="Not a date" errorTitle="Invalid entry" operator="greaterThan" prompt="After 1 Jan 2012. Expected format is YYYY/MM/DD" promptTitle="Please enter a date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:F4" type="date">
       <formula1>40909</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Select a valid instrument from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Instruments' sheet" promptTitle="Select an Instrument" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="list">
-      <formula1>Instruments!$B$4:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -9716,12 +9687,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="6.42914979757085"/>
   </cols>
   <sheetData>
@@ -9854,23 +9825,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6558704453441"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9919,10 +9896,13 @@
       <c r="O1" s="6" t="s">
         <v>764</v>
       </c>
+      <c r="P1" s="6" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="94" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -9980,15 +9960,18 @@
         <v>430</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>769</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="C4" s="79" t="s">
         <v>433</v>
@@ -9998,30 +9981,33 @@
       </c>
       <c r="E4" s="79"/>
       <c r="F4" s="88" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="G4" s="89"/>
       <c r="H4" s="89" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L4" s="93"/>
       <c r="N4" s="40" t="s">
         <v>178</v>
       </c>
       <c r="O4" s="40"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P4" s="0" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="C5" s="79" t="s">
         <v>433</v>
@@ -10031,30 +10017,33 @@
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="88" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="G5" s="89"/>
       <c r="H5" s="89" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L5" s="93"/>
       <c r="N5" s="40" t="s">
         <v>178</v>
       </c>
       <c r="O5" s="40"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P5" s="0" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="C6" s="79" t="s">
         <v>433</v>
@@ -10064,30 +10053,33 @@
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="88" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="G6" s="89"/>
       <c r="H6" s="89" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>30</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L6" s="93"/>
       <c r="N6" s="40" t="s">
         <v>172</v>
       </c>
       <c r="O6" s="40"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P6" s="0" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>783</v>
+        <v>788</v>
       </c>
       <c r="C7" s="79" t="s">
         <v>433</v>
@@ -10097,7 +10089,7 @@
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="88" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="G7" s="89"/>
       <c r="H7" s="89"/>
@@ -10105,7 +10097,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L7" s="93"/>
       <c r="N7" s="40" t="s">
@@ -10113,12 +10105,12 @@
       </c>
       <c r="O7" s="40"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>786</v>
+        <v>791</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>433</v>
@@ -10128,15 +10120,17 @@
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="88" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="G8" s="89"/>
       <c r="H8" s="89" t="s">
-        <v>788</v>
-      </c>
-      <c r="I8" s="5"/>
+        <v>793</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>15</v>
+      </c>
       <c r="J8" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L8" s="93"/>
       <c r="N8" s="40" t="s">
@@ -10146,10 +10140,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>789</v>
+        <v>794</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="C9" s="79" t="s">
         <v>433</v>
@@ -10159,151 +10153,98 @@
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="88" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
       <c r="G9" s="89"/>
       <c r="H9" s="89" t="s">
-        <v>792</v>
+        <v>797</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>10</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L9" s="93"/>
       <c r="N9" s="33" t="s">
         <v>165</v>
       </c>
       <c r="O9" s="40"/>
+      <c r="P9" s="0" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>793</v>
+        <v>799</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>794</v>
+        <v>800</v>
       </c>
       <c r="C10" s="79" t="s">
         <v>433</v>
       </c>
       <c r="D10" s="79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="79"/>
       <c r="F10" s="88" t="s">
-        <v>795</v>
+        <v>801</v>
       </c>
       <c r="G10" s="89"/>
       <c r="H10" s="89" t="s">
-        <v>796</v>
+        <v>802</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L10" s="93"/>
       <c r="N10" s="40" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="O10" s="40"/>
+      <c r="P10" s="0" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>798</v>
+        <v>805</v>
       </c>
       <c r="C11" s="79" t="s">
         <v>433</v>
       </c>
       <c r="D11" s="79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="79"/>
       <c r="F11" s="88" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
       <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
+      <c r="H11" s="89" t="s">
+        <v>807</v>
+      </c>
       <c r="I11" s="5" t="n">
         <v>10</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="L11" s="93"/>
-      <c r="N11" s="40" t="s">
-        <v>178</v>
+      <c r="N11" s="33" t="s">
+        <v>165</v>
       </c>
       <c r="O11" s="40"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>800</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>801</v>
-      </c>
-      <c r="C12" s="79" t="s">
-        <v>433</v>
-      </c>
-      <c r="D12" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="79"/>
-      <c r="F12" s="88" t="s">
-        <v>802</v>
-      </c>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89" t="s">
-        <v>803</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="s">
-        <v>773</v>
-      </c>
-      <c r="L12" s="93"/>
-      <c r="N12" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="O12" s="40"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>804</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>805</v>
-      </c>
-      <c r="C13" s="79" t="s">
-        <v>433</v>
-      </c>
-      <c r="D13" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="79"/>
-      <c r="F13" s="88" t="s">
-        <v>806</v>
-      </c>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89" t="s">
-        <v>807</v>
-      </c>
-      <c r="I13" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>773</v>
-      </c>
-      <c r="L13" s="93"/>
-      <c r="N13" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="O13" s="40"/>
+      <c r="P11" s="0" t="s">
+        <v>808</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10330,10 +10271,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -10351,7 +10292,7 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="14" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C2" s="164"/>
     </row>
@@ -10368,10 +10309,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C4" s="165" t="n">
         <v>0</v>
@@ -10379,10 +10320,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C5" s="165" t="n">
         <v>0</v>
@@ -10390,21 +10331,21 @@
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C6" s="165" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C7" s="166" t="n">
         <v>0</v>
@@ -10412,10 +10353,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C8" s="166" t="n">
         <v>1</v>
@@ -10423,10 +10364,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C9" s="165" t="n">
         <v>15</v>
@@ -10437,7 +10378,7 @@
         <v>498</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C10" s="165" t="n">
         <v>14</v>
@@ -10445,10 +10386,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C11" s="165" t="n">
         <v>5</v>
@@ -10456,10 +10397,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C12" s="165" t="n">
         <v>5</v>
@@ -10467,10 +10408,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C13" s="165" t="n">
         <v>4</v>
@@ -10478,19 +10419,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C14" s="165"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C15" s="166" t="n">
         <v>0</v>
@@ -10498,10 +10439,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C16" s="166" t="n">
         <v>0</v>
@@ -10509,10 +10450,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C17" s="166" t="n">
         <v>1</v>
@@ -10520,22 +10461,22 @@
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C18" s="167" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D18" s="168"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C19" s="169" t="s">
         <v>301</v>
@@ -10544,10 +10485,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C20" s="169" t="s">
         <v>301</v>
@@ -10555,10 +10496,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C21" s="167" t="n">
         <v>30</v>
@@ -10566,10 +10507,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C22" s="167" t="n">
         <v>0</v>
@@ -10577,10 +10518,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C23" s="167" t="n">
         <v>0</v>
@@ -10588,33 +10529,33 @@
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C24" s="169" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D24" s="170"/>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C25" s="169" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C26" s="166" t="n">
         <v>0</v>
@@ -10622,10 +10563,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C27" s="165" t="s">
         <v>597</v>
@@ -10633,10 +10574,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C28" s="165" t="n">
         <v>2</v>
@@ -10644,10 +10585,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C29" s="166" t="n">
         <v>0</v>
@@ -10655,44 +10596,44 @@
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C30" s="165"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C31" s="171" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="24">
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C23" type="whole">
-      <formula1>0</formula1>
-      <formula2>59</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C22" type="whole">
-      <formula1>6</formula1>
-      <formula2>23</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number bigger than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Please enter a whole number bigger than 0" promptTitle="Integer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C21" type="whole">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" error="The number of days before a password expires. 0 disables password expiry" errorTitle="Valid entry" operator="greaterThanOrEqual" prompt="The number of days before a password expires. 0 disables password expiry" promptTitle="Password lifetime" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="The number of minutes before a user is automatically logged off. 0 disables automatic log-off. Must be equal or greater than 0" errorTitle="Invalid entry" operator="greaterThanOrEqual" prompt="The number of minutes of inactivity before a user is automatically logged off. 0 disables automatic log-off" promptTitle="Auto log-off" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5" type="whole">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select a valid entry from the selection list" errorTitle="Invalid entry" operator="equal" prompt="Select a valid currency from the list. Currency codes are maintained on the &quot;Constants&quot; sheet" promptTitle="Currency code" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6" type="list">
+      <formula1>#REF! $B$22:$B$200</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C7 C15:C17 C26 C29" type="list">
+      <formula1>Constants!$G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C8" type="list">
+      <formula1>#REF! $G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Not sure why, must be equal or greater than 0" errorTitle="Invalid entry" operator="between" prompt="The discount percentage entered here, is applied to the prices for clients flagged as 'members', normally co-operative members or associates deserving of this discount" promptTitle="Member discount %" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C9" type="decimal">
@@ -10719,12 +10660,44 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="false" error="Please selct a valid option from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The list is mainatined on the &quot;Constants&quot; sheet" promptTitle="Select an import format from the list" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18" type="list">
+      <formula1>#REF! $C$2:$C$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining moisture. Please select a valid entry from the drop-down menu" promptTitle="Analysis keyword" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18" type="list">
       <formula1>'analysis services'</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid option from the list" promptTitle="File attachments Required, Permitted or Not?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C19:C20" type="list">
+      <formula1>#REF! $D$2:$D$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="'Classic' indicates importing analysis requests per sample and analysis service selection. With 'Profiles', analysis profile keywords are used to select multiple analysis services together" promptTitle="AR Import options" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19" type="list">
+      <formula1>#REF! $B$2:$B$25</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please enter a whole number bigger than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Please enter a whole number bigger than 0" promptTitle="Integer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C21" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C22" type="whole">
+      <formula1>6</formula1>
+      <formula2>23</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C23" type="whole">
+      <formula1>0</formula1>
+      <formula2>59</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 'Register' if you want labels to be automatically printed when new ARs or sample records are created. Select 'Receive' to print labels when ARs or Samples are received. Select 'None' to disable automatic printing" promptTitle="Select a valid option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C24" type="list">
+      <formula1>#REF! $F$2:$F$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The number of days before a sample expires and cannot be analysed any more. This setting can be overwritten per individual sample type  in the sample types setup" promptTitle="Default sample retention period" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D24" type="whole">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select the which label to print when automatic label printing is enabled" promptTitle="Sample label size" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C25" type="list">
+      <formula1>#REF! $E$2:$E$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for Sample IDs. E.g, a water sample will be given an ID of W-0001 if the sample padding was set to 4, and water samples are prefixed with W" promptTitle="Sample ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C27" type="whole">
@@ -10737,38 +10710,6 @@
     </dataValidation>
     <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The full URL: http://URL/path:port" promptTitle="ID Server URL if an external ID server is used" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C30" type="whole">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select a valid entry from the selection list" errorTitle="Invalid entry" operator="equal" prompt="Select a valid currency from the list. Currency codes are maintained on the &quot;Constants&quot; sheet" promptTitle="Currency code" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6" type="list">
-      <formula1>#ref!!$B$22:$B$200</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C8" type="list">
-      <formula1>#ref!!$G$2:$G$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Please selct a valid option from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The list is mainatined on the &quot;Constants&quot; sheet" promptTitle="Select an import format from the list" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18" type="list">
-      <formula1>#ref!!$C$2:$C$4</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid option from the list" promptTitle="File attachments Required, Permitted or Not?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C19:C20" type="list">
-      <formula1>#ref!!$D$2:$D$4</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 'Register' if you want labels to be automatically printed when new ARs or sample records are created. Select 'Receive' to print labels when ARs or Samples are received. Select 'None' to disable automatic printing" promptTitle="Select a valid option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C24" type="list">
-      <formula1>#ref!!$F$2:$F$4</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select the which label to print when automatic label printing is enabled" promptTitle="Sample label size" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C25" type="list">
-      <formula1>#ref!!$E$2:$E$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="'Classic' indicates importing analysis requests per sample and analysis service selection. With 'Profiles', analysis profile keywords are used to select multiple analysis services together" promptTitle="AR Import options" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19" type="list">
-      <formula1>#ref!!$B$2:$B$25</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C7 C15:C17 C26 C29" type="list">
-      <formula1>Constants!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -10816,28 +10757,28 @@
         <v>198</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="G1" s="173" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>511</v>
@@ -10852,63 +10793,63 @@
         <v>243</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="E2" s="174" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="G2" s="51" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>301</v>
       </c>
       <c r="E3" s="174" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="G3" s="51" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="51" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="K3" s="51" t="s">
         <v>535</v>
@@ -10916,19 +10857,19 @@
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>225</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="G4" s="174"/>
       <c r="H4" s="51" t="s">
@@ -10937,28 +10878,28 @@
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="G5" s="174"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="G6" s="174"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="G7" s="174"/>
     </row>
@@ -11020,57 +10961,57 @@
     </row>
     <row r="21" s="178" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="E21" s="177" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="179" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E22" s="174" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="H22" s="51" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="I22" s="51" t="s">
         <v>520</v>
@@ -11078,970 +11019,970 @@
     </row>
     <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="51" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E23" s="174" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="G23" s="51" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="51" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="51" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="H25" s="51" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="51" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="51" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="51" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="51" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="51" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="51" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="51" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="51" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="51" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="51" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="51" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="51" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="51" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="51" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="51" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="51" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="51" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="51" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="51" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="51" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="51" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="51" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="51" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="51" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="51" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="51" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="51" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="51" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="51" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="51" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="51" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="51" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="51" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="51" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="51" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="51" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="51" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="51" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="51" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="51" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="51" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="51" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="51" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="51" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="51" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="51" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="51" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="51" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="51" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="51" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="51" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="51" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="51" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="51" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="51" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="51" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="51" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="51" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="51" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="51" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="51" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="51" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="51" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="51" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="51" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="51" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="51" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="51" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="51" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="51" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="51" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="51" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="51" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="51" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="51" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="51" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="51" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="51" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="51" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="51" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="51" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="51" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="51" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="51" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="51" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="51" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="51" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="51" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="51" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="51" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="51" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="51" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="51" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="51" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="51" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="51" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="51" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="51" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="51" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="51" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="51" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="51" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="51" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="51" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="51" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="51" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="51" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="51" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="51" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="51" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="51" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="51" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="51" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="51" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="51" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="51" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="51" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="51" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="51" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="51" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="51" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="51" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="51" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="51" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="51" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="51" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="51" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="51" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="51" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="51" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="51" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="51" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="51" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="51" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="51" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="51" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="51" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="51" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="51" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="51" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="51" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="51" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="51" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="51" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="51" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="51" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="51" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="51" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="51" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="51" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="51" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="51" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="51" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="51" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="51" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="51" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="51" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="51" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="51" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="51" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="51" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="51" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="51" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="51" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="51" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="51" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="51" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="51" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="51" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="51" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="51" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="51" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="51" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="51" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="51" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -12070,10 +12011,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="28" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -12245,7 +12186,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74898785425101"/>
@@ -12409,16 +12350,16 @@
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get membership discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D8" type="list">
+      <formula1>constaa s $G$2:UG$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" prompt="Enter a number and recognised unit separated by a space, e.g. 100 g or 50 ml" promptTitle="Entry format:" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="F4:F8" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Please enter a whole number greater than or equal to 0" errorTitle="Invalid entry" operator="greaterThanOrEqual" prompt="Please enter a whole number greater than or equal to 0" promptTitle="Integer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C6:C8" type="whole">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get membership discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D8" type="list">
-      <formula1>constaa s!$g$2:ug$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -12450,9 +12391,9 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -12571,12 +12512,12 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation allowBlank="false" error="Select a valid lab contact user name from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Lab Contacts' sheet" promptTitle="Select a valid lab contact (user name)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C7" type="list">
+      <formula1>'Lab Contacts'!$K$4:$K$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid lab contact user name from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Lab Contacts' sheet" promptTitle="Select a valid lab contact (user name)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C8:C26" type="list">
       <formula1>'AR Priorities'!$K$4:$K$30</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Select a valid lab contact user name from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="From the drop-down menu. Maintain the list on the 'Lab Contacts' sheet" promptTitle="Select a valid lab contact (user name)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C7" type="list">
-      <formula1>'Lab Contacts'!$K$4:$K$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -12609,16 +12550,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -13045,8 +12986,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" error="Select a valid option from the drop-down" errorTitle="Invalid group" operator="equal" prompt="The user inherits the autorisation of the groups he/she belongs to. Only add more toles here if you you really need to. Select a valid option from the drop-down" promptTitle="Select additional roles the user needs" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N7" type="list">
-      <formula1>#ref!!$A$2:$A$20</formula1>
+    <dataValidation allowBlank="true" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid Lab Department the staff member belongs to from the drop-down menu" promptTitle="Lab Department" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J4:J7" type="list">
+      <formula1>'Lab Departments'!$A$4:$A$26</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid option from the drop-down" errorTitle="Invalid group" operator="equal" prompt="Select a valid option from the drop-down" promptTitle="Select the autorisation group the user belongs to" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M4:M7" type="list">
@@ -13057,8 +12998,8 @@
       <formula1>Constants!$A$2:$A$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid Lab Department the staff member belongs to from the drop-down menu" promptTitle="Lab Department" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J4:J7" type="list">
-      <formula1>'Lab Departments'!$A$4:$A$26</formula1>
+    <dataValidation allowBlank="false" error="Select a valid option from the drop-down" errorTitle="Invalid group" operator="equal" prompt="The user inherits the autorisation of the groups he/she belongs to. Only add more toles here if you you really need to. Select a valid option from the drop-down" promptTitle="Select additional roles the user needs" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N7" type="list">
+      <formula1>#REF! $A$2:$A$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -13088,13 +13029,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
@@ -13404,21 +13345,17 @@
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="S2:W2"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="M1:M3" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="M4:M5" type="list">
-      <formula1>#ref!!$B$2:$B$1000</formula1>
+  <dataValidations count="3">
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get membership discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C5" type="list">
+      <formula1>Constants!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get bulk discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D5" type="list">
       <formula1>Constants!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get membership discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C5" type="list">
-      <formula1>Constants!$G$2:$G$3</formula1>
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="M4:M5" type="list">
+      <formula1>#REF! $B$2:$B$1000</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -13457,9 +13394,9 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
change import xcel sheet
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/test.xlsx
+++ b/baobab/lims/setupdata/test/test.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="1112">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -2499,7 +2499,7 @@
     <t xml:space="preserve">Def 003</t>
   </si>
   <si>
-    <t xml:space="preserve">Due</t>
+    <t xml:space="preserve">register</t>
   </si>
   <si>
     <t xml:space="preserve">Test Sample 4</t>
@@ -2511,6 +2511,9 @@
     <t xml:space="preserve">Room-2.Freezer-1.Box-01.10</t>
   </si>
   <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 5</t>
   </si>
   <si>
@@ -2547,6 +2550,9 @@
     <t xml:space="preserve">Def 007</t>
   </si>
   <si>
+    <t xml:space="preserve">Receive</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Sample 8</t>
   </si>
   <si>
@@ -2788,9 +2794,6 @@
   </si>
   <si>
     <t xml:space="preserve">Profiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">register</t>
   </si>
   <si>
     <t xml:space="preserve">pdf</t>
@@ -4616,7 +4619,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="112.797570850202"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="114.82995951417"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="6.85425101214575"/>
   </cols>
   <sheetData>
@@ -4686,7 +4689,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.3886639676113"/>
@@ -5004,9 +5007,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="10" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="21" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -5281,11 +5284,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -5458,9 +5461,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5528,7 +5531,7 @@
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5673,12 +5676,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
@@ -5946,11 +5949,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6051,9 +6054,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6144,11 +6147,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -6657,10 +6660,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -6730,12 +6733,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
@@ -7086,8 +7089,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7137,8 +7140,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7191,7 +7194,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -7311,7 +7314,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.5263157894737"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
@@ -7482,9 +7485,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.1295546558704"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -7561,7 +7564,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -7940,11 +7943,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.9919028340081"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
@@ -8180,10 +8183,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="65.7692307692308"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="66.9473684210526"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="96" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8357,8 +8360,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -8429,26 +8432,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8718,8 +8721,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -9113,18 +9116,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="45.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9275,17 +9278,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9428,9 +9431,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -9531,14 +9534,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -9709,12 +9712,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="6.42914979757085"/>
   </cols>
   <sheetData>
@@ -9850,21 +9853,21 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P11" activeCellId="0" sqref="P11"/>
+      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.2429149797571"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9"/>
     <col collapsed="false" hidden="false" max="13" min="9" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="6.63967611336032"/>
@@ -10125,15 +10128,15 @@
       </c>
       <c r="O7" s="40"/>
       <c r="P7" s="0" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>433</v>
@@ -10143,11 +10146,11 @@
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="88" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="G8" s="89"/>
       <c r="H8" s="89" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I8" s="5" t="n">
         <v>15</v>
@@ -10160,16 +10163,13 @@
         <v>178</v>
       </c>
       <c r="O8" s="40"/>
-      <c r="P8" s="0" t="s">
-        <v>776</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C9" s="79" t="s">
         <v>433</v>
@@ -10179,11 +10179,11 @@
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="88" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="G9" s="89"/>
       <c r="H9" s="89" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>10</v>
@@ -10202,10 +10202,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C10" s="79" t="s">
         <v>433</v>
@@ -10215,11 +10215,11 @@
       </c>
       <c r="E10" s="79"/>
       <c r="F10" s="88" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G10" s="89"/>
       <c r="H10" s="89" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="I10" s="5" t="n">
         <v>15</v>
@@ -10233,15 +10233,15 @@
       </c>
       <c r="O10" s="40"/>
       <c r="P10" s="0" t="s">
-        <v>776</v>
+        <v>802</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="C11" s="79" t="s">
         <v>433</v>
@@ -10251,11 +10251,11 @@
       </c>
       <c r="E11" s="79"/>
       <c r="F11" s="88" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="G11" s="89"/>
       <c r="H11" s="89" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="I11" s="5" t="n">
         <v>10</v>
@@ -10268,9 +10268,6 @@
         <v>165</v>
       </c>
       <c r="O11" s="40"/>
-      <c r="P11" s="0" t="s">
-        <v>776</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10297,10 +10294,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -10318,7 +10315,7 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="14" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C2" s="164"/>
     </row>
@@ -10335,10 +10332,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C4" s="165" t="n">
         <v>0</v>
@@ -10346,10 +10343,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="C5" s="165" t="n">
         <v>0</v>
@@ -10357,21 +10354,21 @@
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C6" s="165" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="C7" s="166" t="n">
         <v>0</v>
@@ -10379,10 +10376,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C8" s="166" t="n">
         <v>1</v>
@@ -10390,10 +10387,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C9" s="165" t="n">
         <v>15</v>
@@ -10404,7 +10401,7 @@
         <v>498</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="C10" s="165" t="n">
         <v>14</v>
@@ -10412,10 +10409,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="C11" s="165" t="n">
         <v>5</v>
@@ -10423,10 +10420,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C12" s="165" t="n">
         <v>5</v>
@@ -10434,10 +10431,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="C13" s="165" t="n">
         <v>4</v>
@@ -10445,19 +10442,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="C14" s="165"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="C15" s="166" t="n">
         <v>0</v>
@@ -10465,10 +10462,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C16" s="166" t="n">
         <v>0</v>
@@ -10476,10 +10473,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C17" s="166" t="n">
         <v>1</v>
@@ -10487,22 +10484,22 @@
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="C18" s="167" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="D18" s="168"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C19" s="169" t="s">
         <v>301</v>
@@ -10511,10 +10508,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="C20" s="169" t="s">
         <v>301</v>
@@ -10522,10 +10519,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="C21" s="167" t="n">
         <v>30</v>
@@ -10533,10 +10530,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="C22" s="167" t="n">
         <v>0</v>
@@ -10544,10 +10541,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="C23" s="167" t="n">
         <v>0</v>
@@ -10555,33 +10552,33 @@
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="C24" s="169" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="D24" s="170"/>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="C25" s="169" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="C26" s="166" t="n">
         <v>0</v>
@@ -10589,10 +10586,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C27" s="165" t="s">
         <v>597</v>
@@ -10600,10 +10597,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="C28" s="165" t="n">
         <v>2</v>
@@ -10611,10 +10608,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="C29" s="166" t="n">
         <v>0</v>
@@ -10622,22 +10619,22 @@
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="C30" s="165"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="C31" s="171" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
     </row>
   </sheetData>
@@ -10783,28 +10780,28 @@
         <v>198</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="G1" s="173" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>511</v>
@@ -10819,63 +10816,63 @@
         <v>243</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="E2" s="174" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="G2" s="51" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="K2" s="51" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>301</v>
       </c>
       <c r="E3" s="174" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>882</v>
+        <v>785</v>
       </c>
       <c r="G3" s="51" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="51" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="K3" s="51" t="s">
         <v>535</v>
@@ -10883,19 +10880,19 @@
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>225</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="G4" s="174"/>
       <c r="H4" s="51" t="s">
@@ -10904,28 +10901,28 @@
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="51" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="G5" s="174"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="G6" s="174"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="G7" s="174"/>
     </row>
@@ -10987,57 +10984,57 @@
     </row>
     <row r="21" s="178" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E21" s="177" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="179" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="E22" s="174" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="H22" s="51" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="I22" s="51" t="s">
         <v>520</v>
@@ -11045,970 +11042,970 @@
     </row>
     <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="51" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="E23" s="174" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="G23" s="51" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="H23" s="51" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="51" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="51" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="H25" s="51" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="51" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="51" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="51" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="51" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="51" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="51" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="51" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="51" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="51" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="51" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="51" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="51" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="51" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="51" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="51" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="51" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="51" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="51" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="51" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="51" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="51" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="51" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="51" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="51" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="51" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="51" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="51" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="51" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="51" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="51" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="51" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="51" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="51" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="51" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="51" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="51" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="51" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="51" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="51" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="51" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="51" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="51" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="51" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="51" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="51" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="51" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="51" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="51" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="51" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="51" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="51" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="51" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="51" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="51" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="51" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="51" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="51" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="51" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="51" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="51" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="51" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="51" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="51" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="51" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="51" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="51" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="51" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="51" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="51" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="51" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="51" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="51" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="51" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="51" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="51" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="51" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="51" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="51" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="51" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="51" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="51" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="51" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="51" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="51" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="51" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="51" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="51" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="51" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="51" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="51" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="51" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="51" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="51" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="51" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="51" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="51" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="51" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="51" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="51" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="51" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="51" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="51" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="51" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="51" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="51" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="51" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="51" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="51" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="51" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="51" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="51" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="51" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="51" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="51" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="51" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="51" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="51" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="51" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="51" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="51" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="51" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="51" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="51" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="51" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="51" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="51" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="51" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="51" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="51" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="51" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="51" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="51" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="51" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="51" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="51" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="51" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="51" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="51" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="51" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="51" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="51" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="51" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="51" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="51" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="51" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="51" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="51" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="51" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="51" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="51" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="51" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="51" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="51" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="51" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="51" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="51" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="51" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="51" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="51" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="51" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="51" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="51" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="51" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="51" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="51" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="51" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="51" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="51" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="51" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="51" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="51" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="51" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="51" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="51" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="51" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
   </sheetData>
@@ -12039,8 +12036,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="28" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -12212,7 +12209,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74898785425101"/>
@@ -12417,7 +12414,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
@@ -12576,7 +12573,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
@@ -12585,7 +12582,7 @@
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="35.1336032388664"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -13055,13 +13052,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
@@ -13424,9 +13421,9 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
Git add MACAddress on importer
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/test.xlsx
+++ b/baobab/lims/setupdata/test/test.xlsx
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="1348">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -3572,6 +3572,9 @@
     <t xml:space="preserve">ZWL</t>
   </si>
   <si>
+    <t xml:space="preserve">MACAddress</t>
+  </si>
+  <si>
     <t xml:space="preserve">MonitoringDevices</t>
   </si>
   <si>
@@ -3581,7 +3584,13 @@
     <t xml:space="preserve">Temperature Monitoring Device</t>
   </si>
   <si>
+    <t xml:space="preserve"> 98:8B:AD:28:04:26</t>
+  </si>
+  <si>
     <t xml:space="preserve">Device 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test mac address</t>
   </si>
   <si>
     <t xml:space="preserve">MonitoringDevice</t>
@@ -4228,7 +4237,7 @@
     <numFmt numFmtId="170" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="171" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4475,12 +4484,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -4561,7 +4564,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="183">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5284,10 +5287,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -5450,7 +5449,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.39"/>
@@ -5767,7 +5766,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="8.14"/>
@@ -6043,7 +6042,7 @@
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.02"/>
@@ -6219,7 +6218,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.02"/>
@@ -6417,7 +6416,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.02"/>
@@ -6577,7 +6576,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.21"/>
@@ -6643,7 +6642,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.39"/>
@@ -7060,7 +7059,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.71"/>
@@ -7165,7 +7164,7 @@
       <selection pane="topLeft" activeCell="W22" activeCellId="0" sqref="W22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.89"/>
@@ -8125,7 +8124,7 @@
       <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.89"/>
@@ -8196,7 +8195,7 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.92"/>
@@ -8246,7 +8245,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.49"/>
@@ -8296,7 +8295,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.68"/>
@@ -8417,7 +8416,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.43"/>
@@ -8587,7 +8586,7 @@
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.33203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.3359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.95"/>
@@ -8665,7 +8664,7 @@
       <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="26.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="7.51"/>
@@ -9279,7 +9278,7 @@
       <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="62.45"/>
@@ -9922,7 +9921,7 @@
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.91"/>
@@ -10519,7 +10518,7 @@
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.39"/>
@@ -11355,7 +11354,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.78"/>
@@ -11823,7 +11822,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.38671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.89"/>
@@ -13265,7 +13264,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13286,7 +13285,9 @@
       <c r="B1" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="7" t="s">
+        <v>1131</v>
+      </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -13296,7 +13297,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="94" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -13313,7 +13314,9 @@
       <c r="B3" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>1131</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -13323,12 +13326,14 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C4" s="79"/>
+        <v>1134</v>
+      </c>
+      <c r="C4" s="79" t="s">
+        <v>1135</v>
+      </c>
       <c r="D4" s="97"/>
       <c r="E4" s="88"/>
       <c r="F4" s="162"/>
@@ -13338,12 +13343,14 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>1134</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>1133</v>
-      </c>
-      <c r="C5" s="79"/>
+      <c r="C5" s="79" t="s">
+        <v>1137</v>
+      </c>
       <c r="D5" s="97"/>
       <c r="F5" s="162"/>
     </row>
@@ -13369,7 +13376,7 @@
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.13"/>
@@ -13386,7 +13393,7 @@
         <v>478</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -13396,7 +13403,7 @@
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="94" t="s">
-        <v>1136</v>
+        <v>1139</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -13417,7 +13424,7 @@
         <v>478</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -13430,13 +13437,13 @@
         <v>483</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1137</v>
+        <v>1140</v>
       </c>
       <c r="C4" s="79" t="s">
         <v>483</v>
       </c>
       <c r="D4" s="97" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="E4" s="88"/>
       <c r="F4" s="162"/>
@@ -13466,13 +13473,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F100" activeCellId="0" sqref="F100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="180" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.29"/>
@@ -13483,2277 +13490,2061 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="126" t="s">
-        <v>1138</v>
+        <v>1141</v>
       </c>
       <c r="B1" s="94" t="s">
-        <v>1139</v>
+        <v>1142</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>399</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>1141</v>
+        <v>1144</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1142</v>
-      </c>
-      <c r="G1" s="181" t="s">
-        <v>1135</v>
+        <v>1145</v>
+      </c>
+      <c r="G1" s="97" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="126" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="29"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="182" t="s">
-        <v>1138</v>
+      <c r="A3" s="181" t="s">
+        <v>1141</v>
       </c>
       <c r="B3" s="97" t="s">
-        <v>1139</v>
+        <v>1142</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>399</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1141</v>
+        <v>1144</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1142</v>
+        <v>1145</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="183" t="s">
-        <v>1144</v>
+      <c r="A4" s="182" t="s">
+        <v>1147</v>
       </c>
       <c r="B4" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="C4" s="79" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1147</v>
+        <v>1150</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="183" t="s">
+      <c r="A5" s="182" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B5" s="97" t="s">
         <v>1148</v>
       </c>
-      <c r="B5" s="97" t="s">
-        <v>1145</v>
-      </c>
       <c r="D5" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1149</v>
+        <v>1152</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="183" t="s">
-        <v>1150</v>
+      <c r="A6" s="182" t="s">
+        <v>1153</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D6" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1151</v>
+        <v>1154</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="183" t="s">
-        <v>1152</v>
+      <c r="A7" s="182" t="s">
+        <v>1155</v>
       </c>
       <c r="B7" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D7" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1153</v>
+        <v>1156</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="183" t="s">
-        <v>1154</v>
+      <c r="A8" s="182" t="s">
+        <v>1157</v>
       </c>
       <c r="B8" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D8" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>1155</v>
+        <v>1158</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="183" t="s">
-        <v>1156</v>
+      <c r="A9" s="182" t="s">
+        <v>1159</v>
       </c>
       <c r="B9" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D9" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>1157</v>
+        <v>1160</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="183" t="s">
-        <v>1158</v>
+      <c r="A10" s="182" t="s">
+        <v>1161</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D10" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>1159</v>
+        <v>1162</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="183" t="s">
-        <v>1160</v>
+      <c r="A11" s="182" t="s">
+        <v>1163</v>
       </c>
       <c r="B11" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D11" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="183" t="s">
-        <v>1162</v>
+      <c r="A12" s="182" t="s">
+        <v>1165</v>
       </c>
       <c r="B12" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D12" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>1163</v>
+        <v>1166</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="183" t="s">
-        <v>1164</v>
+      <c r="A13" s="182" t="s">
+        <v>1167</v>
       </c>
       <c r="B13" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D13" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>1165</v>
+        <v>1168</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="183" t="s">
-        <v>1166</v>
+      <c r="A14" s="182" t="s">
+        <v>1169</v>
       </c>
       <c r="B14" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D14" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>1167</v>
+        <v>1170</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="183" t="s">
-        <v>1168</v>
+      <c r="A15" s="182" t="s">
+        <v>1171</v>
       </c>
       <c r="B15" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D15" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>1169</v>
+        <v>1172</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="183" t="s">
-        <v>1170</v>
+      <c r="A16" s="182" t="s">
+        <v>1173</v>
       </c>
       <c r="B16" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D16" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>1171</v>
+        <v>1174</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="183" t="s">
-        <v>1172</v>
+      <c r="A17" s="182" t="s">
+        <v>1175</v>
       </c>
       <c r="B17" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D17" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>1173</v>
+        <v>1176</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="183" t="s">
-        <v>1174</v>
+      <c r="A18" s="182" t="s">
+        <v>1177</v>
       </c>
       <c r="B18" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D18" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>1175</v>
+        <v>1178</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="183" t="s">
-        <v>1176</v>
+      <c r="A19" s="182" t="s">
+        <v>1179</v>
       </c>
       <c r="B19" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D19" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>1177</v>
+        <v>1180</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="183" t="s">
-        <v>1178</v>
+      <c r="A20" s="182" t="s">
+        <v>1181</v>
       </c>
       <c r="B20" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D20" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>1179</v>
+        <v>1182</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="183" t="s">
-        <v>1180</v>
+      <c r="A21" s="182" t="s">
+        <v>1183</v>
       </c>
       <c r="B21" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D21" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>1181</v>
+        <v>1184</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="183" t="s">
-        <v>1182</v>
+      <c r="A22" s="182" t="s">
+        <v>1185</v>
       </c>
       <c r="B22" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D22" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>1183</v>
+        <v>1186</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="183" t="s">
-        <v>1184</v>
+      <c r="A23" s="182" t="s">
+        <v>1187</v>
       </c>
       <c r="B23" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D23" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>1185</v>
+        <v>1188</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="183" t="s">
-        <v>1186</v>
+      <c r="A24" s="182" t="s">
+        <v>1189</v>
       </c>
       <c r="B24" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D24" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>1187</v>
+        <v>1190</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="183" t="s">
-        <v>1188</v>
+      <c r="A25" s="182" t="s">
+        <v>1191</v>
       </c>
       <c r="B25" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D25" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>1189</v>
+        <v>1192</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="183" t="s">
-        <v>1190</v>
+      <c r="A26" s="182" t="s">
+        <v>1193</v>
       </c>
       <c r="B26" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D26" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>1191</v>
+        <v>1194</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="183" t="s">
-        <v>1192</v>
+      <c r="A27" s="182" t="s">
+        <v>1195</v>
       </c>
       <c r="B27" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D27" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="183" t="s">
-        <v>1194</v>
+      <c r="A28" s="182" t="s">
+        <v>1197</v>
       </c>
       <c r="B28" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D28" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="183" t="s">
-        <v>1196</v>
+      <c r="A29" s="182" t="s">
+        <v>1199</v>
       </c>
       <c r="B29" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D29" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="183" t="s">
-        <v>1198</v>
+      <c r="A30" s="182" t="s">
+        <v>1201</v>
       </c>
       <c r="B30" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D30" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>1199</v>
+        <v>1202</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="183" t="s">
-        <v>1200</v>
+      <c r="A31" s="182" t="s">
+        <v>1203</v>
       </c>
       <c r="B31" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D31" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>1201</v>
+        <v>1204</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="183" t="s">
-        <v>1202</v>
+      <c r="A32" s="182" t="s">
+        <v>1205</v>
       </c>
       <c r="B32" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D32" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>1203</v>
+        <v>1206</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="183" t="s">
-        <v>1204</v>
+      <c r="A33" s="182" t="s">
+        <v>1207</v>
       </c>
       <c r="B33" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D33" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>1205</v>
+        <v>1208</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="183" t="s">
-        <v>1206</v>
+      <c r="A34" s="182" t="s">
+        <v>1209</v>
       </c>
       <c r="B34" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D34" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="183" t="s">
-        <v>1208</v>
+      <c r="A35" s="182" t="s">
+        <v>1211</v>
       </c>
       <c r="B35" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D35" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>1209</v>
+        <v>1212</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="183" t="s">
-        <v>1210</v>
+      <c r="A36" s="182" t="s">
+        <v>1213</v>
       </c>
       <c r="B36" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D36" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>1211</v>
+        <v>1214</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="183" t="s">
-        <v>1212</v>
+      <c r="A37" s="182" t="s">
+        <v>1215</v>
       </c>
       <c r="B37" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D37" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>1213</v>
+        <v>1216</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="183" t="s">
-        <v>1214</v>
+      <c r="A38" s="182" t="s">
+        <v>1217</v>
       </c>
       <c r="B38" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D38" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>1215</v>
+        <v>1218</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="183" t="s">
-        <v>1216</v>
+      <c r="A39" s="182" t="s">
+        <v>1219</v>
       </c>
       <c r="B39" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D39" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>1217</v>
+        <v>1220</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="183" t="s">
-        <v>1218</v>
+      <c r="A40" s="182" t="s">
+        <v>1221</v>
       </c>
       <c r="B40" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D40" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>1219</v>
+        <v>1222</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="183" t="s">
-        <v>1220</v>
+      <c r="A41" s="182" t="s">
+        <v>1223</v>
       </c>
       <c r="B41" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D41" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>1221</v>
+        <v>1224</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="183" t="s">
-        <v>1222</v>
+      <c r="A42" s="182" t="s">
+        <v>1225</v>
       </c>
       <c r="B42" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D42" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>1223</v>
+        <v>1226</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="183" t="s">
-        <v>1224</v>
+      <c r="A43" s="182" t="s">
+        <v>1227</v>
       </c>
       <c r="B43" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D43" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>1225</v>
+        <v>1228</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="183" t="s">
-        <v>1226</v>
+      <c r="A44" s="182" t="s">
+        <v>1229</v>
       </c>
       <c r="B44" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D44" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>1227</v>
+        <v>1230</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="183" t="s">
-        <v>1228</v>
+      <c r="A45" s="182" t="s">
+        <v>1231</v>
       </c>
       <c r="B45" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D45" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>1229</v>
+        <v>1232</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="183" t="s">
-        <v>1230</v>
+      <c r="A46" s="182" t="s">
+        <v>1233</v>
       </c>
       <c r="B46" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D46" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>1231</v>
+        <v>1234</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="183" t="s">
-        <v>1232</v>
+      <c r="A47" s="182" t="s">
+        <v>1235</v>
       </c>
       <c r="B47" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D47" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>1233</v>
+        <v>1236</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="183" t="s">
-        <v>1234</v>
+      <c r="A48" s="182" t="s">
+        <v>1237</v>
       </c>
       <c r="B48" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D48" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="183" t="s">
-        <v>1236</v>
+      <c r="A49" s="182" t="s">
+        <v>1239</v>
       </c>
       <c r="B49" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D49" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>1237</v>
+        <v>1240</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="183" t="s">
-        <v>1238</v>
+      <c r="A50" s="182" t="s">
+        <v>1241</v>
       </c>
       <c r="B50" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D50" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>1239</v>
+        <v>1242</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="183" t="s">
-        <v>1240</v>
+      <c r="A51" s="182" t="s">
+        <v>1243</v>
       </c>
       <c r="B51" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D51" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>1241</v>
+        <v>1244</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="183" t="s">
-        <v>1242</v>
+      <c r="A52" s="182" t="s">
+        <v>1245</v>
       </c>
       <c r="B52" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D52" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>1243</v>
+        <v>1246</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="183" t="s">
-        <v>1244</v>
+      <c r="A53" s="182" t="s">
+        <v>1247</v>
       </c>
       <c r="B53" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D53" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>1245</v>
+        <v>1248</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="183" t="s">
-        <v>1246</v>
+      <c r="A54" s="182" t="s">
+        <v>1249</v>
       </c>
       <c r="B54" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D54" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>1247</v>
+        <v>1250</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="183" t="s">
-        <v>1248</v>
+      <c r="A55" s="182" t="s">
+        <v>1251</v>
       </c>
       <c r="B55" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D55" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>1249</v>
+        <v>1252</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="183" t="s">
-        <v>1250</v>
+      <c r="A56" s="182" t="s">
+        <v>1253</v>
       </c>
       <c r="B56" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D56" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="183" t="s">
-        <v>1252</v>
+      <c r="A57" s="182" t="s">
+        <v>1255</v>
       </c>
       <c r="B57" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D57" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="183" t="s">
-        <v>1254</v>
+      <c r="A58" s="182" t="s">
+        <v>1257</v>
       </c>
       <c r="B58" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D58" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>1255</v>
+        <v>1258</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="183" t="s">
-        <v>1256</v>
+      <c r="A59" s="182" t="s">
+        <v>1259</v>
       </c>
       <c r="B59" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D59" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>1257</v>
+        <v>1260</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="183" t="s">
-        <v>1258</v>
+      <c r="A60" s="182" t="s">
+        <v>1261</v>
       </c>
       <c r="B60" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D60" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>1259</v>
+        <v>1262</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="183" t="s">
-        <v>1260</v>
+      <c r="A61" s="182" t="s">
+        <v>1263</v>
       </c>
       <c r="B61" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D61" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>1261</v>
+        <v>1264</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="183" t="s">
-        <v>1262</v>
+      <c r="A62" s="182" t="s">
+        <v>1265</v>
       </c>
       <c r="B62" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D62" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="F62" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="183" t="s">
-        <v>1264</v>
+      <c r="A63" s="182" t="s">
+        <v>1267</v>
       </c>
       <c r="B63" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D63" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>1265</v>
+        <v>1268</v>
       </c>
       <c r="F63" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="183" t="s">
-        <v>1266</v>
+      <c r="A64" s="182" t="s">
+        <v>1269</v>
       </c>
       <c r="B64" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D64" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="183" t="s">
-        <v>1268</v>
+      <c r="A65" s="182" t="s">
+        <v>1271</v>
       </c>
       <c r="B65" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D65" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>1269</v>
+        <v>1272</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="183" t="s">
-        <v>1270</v>
+      <c r="A66" s="182" t="s">
+        <v>1273</v>
       </c>
       <c r="B66" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D66" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>1271</v>
+        <v>1274</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="183" t="s">
-        <v>1272</v>
+      <c r="A67" s="182" t="s">
+        <v>1275</v>
       </c>
       <c r="B67" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D67" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>1273</v>
+        <v>1276</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="183" t="s">
-        <v>1274</v>
+      <c r="A68" s="182" t="s">
+        <v>1277</v>
       </c>
       <c r="B68" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D68" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="183" t="s">
-        <v>1276</v>
+      <c r="A69" s="182" t="s">
+        <v>1279</v>
       </c>
       <c r="B69" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D69" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>1277</v>
+        <v>1280</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="183" t="s">
-        <v>1278</v>
+      <c r="A70" s="182" t="s">
+        <v>1281</v>
       </c>
       <c r="B70" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D70" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>1279</v>
+        <v>1282</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="183" t="s">
-        <v>1280</v>
+      <c r="A71" s="182" t="s">
+        <v>1283</v>
       </c>
       <c r="B71" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D71" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>1281</v>
+        <v>1284</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="183" t="s">
-        <v>1282</v>
+      <c r="A72" s="182" t="s">
+        <v>1285</v>
       </c>
       <c r="B72" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D72" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>1283</v>
+        <v>1286</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="183" t="s">
-        <v>1284</v>
+      <c r="A73" s="182" t="s">
+        <v>1287</v>
       </c>
       <c r="B73" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D73" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>1285</v>
+        <v>1288</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="183" t="s">
-        <v>1286</v>
+      <c r="A74" s="182" t="s">
+        <v>1289</v>
       </c>
       <c r="B74" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D74" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>1287</v>
+        <v>1290</v>
       </c>
       <c r="F74" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="183" t="s">
-        <v>1288</v>
+      <c r="A75" s="182" t="s">
+        <v>1291</v>
       </c>
       <c r="B75" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D75" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>1289</v>
+        <v>1292</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="183" t="s">
-        <v>1290</v>
+      <c r="A76" s="182" t="s">
+        <v>1293</v>
       </c>
       <c r="B76" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D76" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>1291</v>
+        <v>1294</v>
       </c>
       <c r="F76" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="183" t="s">
-        <v>1292</v>
+      <c r="A77" s="182" t="s">
+        <v>1295</v>
       </c>
       <c r="B77" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D77" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>1293</v>
+        <v>1296</v>
       </c>
       <c r="F77" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="183" t="s">
-        <v>1294</v>
+      <c r="A78" s="182" t="s">
+        <v>1297</v>
       </c>
       <c r="B78" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D78" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>1295</v>
+        <v>1298</v>
       </c>
       <c r="F78" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="183" t="s">
-        <v>1296</v>
+      <c r="A79" s="182" t="s">
+        <v>1299</v>
       </c>
       <c r="B79" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D79" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>1297</v>
+        <v>1300</v>
       </c>
       <c r="F79" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="183" t="s">
-        <v>1298</v>
+      <c r="A80" s="182" t="s">
+        <v>1301</v>
       </c>
       <c r="B80" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D80" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>1299</v>
+        <v>1302</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="183" t="s">
-        <v>1300</v>
+      <c r="A81" s="182" t="s">
+        <v>1303</v>
       </c>
       <c r="B81" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D81" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>1301</v>
+        <v>1304</v>
       </c>
       <c r="F81" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="183" t="s">
-        <v>1302</v>
+      <c r="A82" s="182" t="s">
+        <v>1305</v>
       </c>
       <c r="B82" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D82" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>1303</v>
+        <v>1306</v>
       </c>
       <c r="F82" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="183" t="s">
-        <v>1304</v>
+      <c r="A83" s="182" t="s">
+        <v>1307</v>
       </c>
       <c r="B83" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D83" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>1305</v>
+        <v>1308</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="183" t="s">
-        <v>1306</v>
+      <c r="A84" s="182" t="s">
+        <v>1309</v>
       </c>
       <c r="B84" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D84" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>1307</v>
+        <v>1310</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="183" t="s">
-        <v>1308</v>
+      <c r="A85" s="182" t="s">
+        <v>1311</v>
       </c>
       <c r="B85" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D85" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>1309</v>
+        <v>1312</v>
       </c>
       <c r="F85" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="183" t="s">
-        <v>1310</v>
+      <c r="A86" s="182" t="s">
+        <v>1313</v>
       </c>
       <c r="B86" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D86" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>1311</v>
+        <v>1314</v>
       </c>
       <c r="F86" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="183" t="s">
-        <v>1312</v>
+      <c r="A87" s="182" t="s">
+        <v>1315</v>
       </c>
       <c r="B87" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D87" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>1313</v>
+        <v>1316</v>
       </c>
       <c r="F87" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="183" t="s">
-        <v>1314</v>
+      <c r="A88" s="182" t="s">
+        <v>1317</v>
       </c>
       <c r="B88" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D88" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="F88" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="183" t="s">
-        <v>1316</v>
+      <c r="A89" s="182" t="s">
+        <v>1319</v>
       </c>
       <c r="B89" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D89" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>1317</v>
+        <v>1320</v>
       </c>
       <c r="F89" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="183" t="s">
-        <v>1318</v>
+      <c r="A90" s="182" t="s">
+        <v>1321</v>
       </c>
       <c r="B90" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D90" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>1319</v>
+        <v>1322</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="183" t="s">
-        <v>1320</v>
+      <c r="A91" s="182" t="s">
+        <v>1323</v>
       </c>
       <c r="B91" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D91" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>1321</v>
+        <v>1324</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="183" t="s">
-        <v>1322</v>
+      <c r="A92" s="182" t="s">
+        <v>1325</v>
       </c>
       <c r="B92" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D92" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>1323</v>
+        <v>1326</v>
       </c>
       <c r="F92" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="183" t="s">
-        <v>1324</v>
+      <c r="A93" s="182" t="s">
+        <v>1327</v>
       </c>
       <c r="B93" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D93" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>1325</v>
+        <v>1328</v>
       </c>
       <c r="F93" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="183" t="s">
-        <v>1324</v>
+      <c r="A94" s="182" t="s">
+        <v>1327</v>
       </c>
       <c r="B94" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D94" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>1326</v>
+        <v>1329</v>
       </c>
       <c r="F94" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="183" t="s">
-        <v>1327</v>
+      <c r="A95" s="182" t="s">
+        <v>1330</v>
       </c>
       <c r="B95" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D95" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>1328</v>
+        <v>1331</v>
       </c>
       <c r="F95" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="183" t="s">
-        <v>1329</v>
+      <c r="A96" s="182" t="s">
+        <v>1332</v>
       </c>
       <c r="B96" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D96" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>1330</v>
+        <v>1333</v>
       </c>
       <c r="F96" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="183" t="s">
-        <v>1331</v>
+      <c r="A97" s="182" t="s">
+        <v>1334</v>
       </c>
       <c r="B97" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D97" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>1332</v>
+        <v>1335</v>
       </c>
       <c r="F97" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="183" t="s">
-        <v>1333</v>
+      <c r="A98" s="182" t="s">
+        <v>1336</v>
       </c>
       <c r="B98" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D98" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>1334</v>
+        <v>1337</v>
       </c>
       <c r="F98" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="183" t="s">
-        <v>1335</v>
+      <c r="A99" s="182" t="s">
+        <v>1338</v>
       </c>
       <c r="B99" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D99" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>1336</v>
+        <v>1339</v>
       </c>
       <c r="F99" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="183" t="s">
-        <v>1337</v>
+      <c r="A100" s="182" t="s">
+        <v>1340</v>
       </c>
       <c r="B100" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D100" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>1338</v>
+        <v>1341</v>
       </c>
       <c r="F100" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="183" t="s">
-        <v>1339</v>
+      <c r="A101" s="182" t="s">
+        <v>1342</v>
       </c>
       <c r="B101" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D101" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>1340</v>
+        <v>1343</v>
       </c>
       <c r="F101" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="183" t="s">
-        <v>1341</v>
+      <c r="A102" s="182" t="s">
+        <v>1344</v>
       </c>
       <c r="B102" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D102" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>1342</v>
+        <v>1345</v>
       </c>
       <c r="F102" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="183" t="s">
-        <v>1343</v>
+      <c r="A103" s="182" t="s">
+        <v>1346</v>
       </c>
       <c r="B103" s="97" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="D103" s="97" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>1344</v>
+        <v>1347</v>
       </c>
       <c r="F103" s="0" t="s">
         <v>483</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D104" s="97"/>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D105" s="97"/>
-    </row>
-    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>1133</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -15978,7 +15769,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.96"/>
@@ -16973,7 +16764,7 @@
       <selection pane="topLeft" activeCell="R16" activeCellId="0" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.96"/>

</xml_diff>

<commit_message>
Fix import donor sex
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/test.xlsx
+++ b/baobab/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="36"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,10 +20,10 @@
     <sheet name="Suppliers" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Supplier Contacts" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Products" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Donor" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="DiseaseOntology" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Kit Templates" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Projects" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="DiseaseOntology" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Kit Templates" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Projects" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Donor" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Storage" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Kit Components" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Analysis Categories" sheetId="19" state="visible" r:id="rId20"/>
@@ -1382,63 +1382,6 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">SampleDonorID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SelectedProject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgeUnit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green Goblin Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Version</t>
   </si>
   <si>
@@ -1574,6 +1517,9 @@
     <t xml:space="preserve">Date Crated</t>
   </si>
   <si>
+    <t xml:space="preserve">Green Goblin Project</t>
+  </si>
+  <si>
     <t xml:space="preserve">Development of serum which gives superhuman strength and intelligence</t>
   </si>
   <si>
@@ -1593,6 +1539,60 @@
   </si>
   <si>
     <t xml:space="preserve">2012/06/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleDonorID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SelectedProject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgeUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
   </si>
   <si>
     <t xml:space="preserve">hierarchy</t>
@@ -5412,7 +5412,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="108.939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="109.902834008097"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="6.85425101214575"/>
   </cols>
   <sheetData>
@@ -5482,7 +5482,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.497975708502"/>
@@ -5800,9 +5800,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="10" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="21" min="12" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -6077,11 +6077,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -6246,38 +6246,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>413</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>415</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
@@ -6318,19 +6318,19 @@
     </row>
     <row r="3" s="7" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>413</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>415</v>
       </c>
       <c r="ALW3" s="0"/>
       <c r="ALX3" s="0"/>
@@ -6349,83 +6349,45 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="79" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4" s="88" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>410</v>
+      </c>
+      <c r="D4" s="89" t="s">
         <v>416</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="E4" s="88" t="s">
         <v>417</v>
-      </c>
-      <c r="C4" s="89" t="s">
-        <v>418</v>
-      </c>
-      <c r="D4" s="89" t="s">
-        <v>419</v>
-      </c>
-      <c r="E4" s="88" t="s">
-        <v>420</v>
       </c>
       <c r="F4" s="83"/>
       <c r="G4" s="90"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="79" t="s">
-        <v>421</v>
-      </c>
-      <c r="B5" s="79" t="s">
-        <v>417</v>
+        <v>418</v>
+      </c>
+      <c r="B5" s="88" t="s">
+        <v>419</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="D5" s="89" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F5" s="83"/>
       <c r="G5" s="90"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="79" t="s">
-        <v>425</v>
-      </c>
-      <c r="B6" s="79" t="s">
-        <v>417</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>426</v>
-      </c>
-      <c r="D6" s="89" t="s">
-        <v>427</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="90"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="79" t="s">
-        <v>428</v>
-      </c>
-      <c r="B7" s="79" t="s">
-        <v>417</v>
-      </c>
-      <c r="C7" s="89" t="s">
-        <v>418</v>
-      </c>
-      <c r="D7" s="89" t="s">
-        <v>429</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="90"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" prompt="Please select a valid Suppliers  the staff member belongs to from the drop-down menu" promptTitle="Suppliers" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4:F7" type="list">
+    <dataValidation allowBlank="true" operator="equal" prompt="Please select a valid Suppliers  the staff member belongs to from the drop-down menu" promptTitle="Suppliers" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4:F5" type="list">
       <formula1>Suppliers!$A$4:$A$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6445,38 +6407,253 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="91" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="91" t="s">
+        <v>421</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>423</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="92" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="3" s="52" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="52" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>426</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>401</v>
+      </c>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="29"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="79" t="s">
+        <v>446</v>
+      </c>
+      <c r="B4" s="79" t="s">
+        <v>447</v>
+      </c>
+      <c r="C4" s="79" t="s">
+        <v>448</v>
+      </c>
+      <c r="D4" s="88" t="n">
+        <v>34</v>
+      </c>
+      <c r="E4" s="89" t="s">
+        <v>449</v>
+      </c>
+      <c r="F4" s="89" t="s">
+        <v>450</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="J4" s="93" t="s">
+        <v>453</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>133</v>
+        <v>454</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>134</v>
+        <v>455</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>431</v>
+        <v>457</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>432</v>
+        <v>458</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
@@ -6517,19 +6694,19 @@
     </row>
     <row r="3" s="7" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>133</v>
+        <v>454</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>455</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>431</v>
+        <v>457</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>432</v>
+        <v>458</v>
       </c>
       <c r="ALW3" s="0"/>
       <c r="ALX3" s="0"/>
@@ -6548,264 +6725,87 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="79" t="s">
-        <v>433</v>
-      </c>
-      <c r="B4" s="88" t="s">
-        <v>434</v>
+        <v>459</v>
+      </c>
+      <c r="B4" s="79" t="s">
+        <v>446</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>410</v>
+        <v>460</v>
       </c>
       <c r="D4" s="89" t="s">
-        <v>435</v>
+        <v>461</v>
       </c>
       <c r="E4" s="88" t="s">
-        <v>436</v>
+        <v>462</v>
       </c>
       <c r="F4" s="83"/>
       <c r="G4" s="90"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="79" t="s">
-        <v>437</v>
-      </c>
-      <c r="B5" s="88" t="s">
-        <v>438</v>
+        <v>463</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>446</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>410</v>
+        <v>464</v>
       </c>
       <c r="D5" s="89" t="s">
-        <v>437</v>
+        <v>465</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>439</v>
+        <v>466</v>
       </c>
       <c r="F5" s="83"/>
       <c r="G5" s="90"/>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="79" t="s">
+        <v>467</v>
+      </c>
+      <c r="B6" s="79" t="s">
+        <v>446</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>468</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>469</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="F6" s="83"/>
+      <c r="G6" s="90"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="79" t="s">
+        <v>470</v>
+      </c>
+      <c r="B7" s="79" t="s">
+        <v>446</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>460</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>471</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="F7" s="83"/>
+      <c r="G7" s="90"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" prompt="Please select a valid Suppliers  the staff member belongs to from the drop-down menu" promptTitle="Suppliers" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4:F5" type="list">
+    <dataValidation allowBlank="true" operator="equal" prompt="Please select a valid Suppliers  the staff member belongs to from the drop-down menu" promptTitle="Suppliers" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4:F7" type="list">
       <formula1>Suppliers!$A$4:$A$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="91" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="91" t="s">
-        <v>440</v>
-      </c>
-      <c r="B1" s="91" t="s">
-        <v>441</v>
-      </c>
-      <c r="C1" s="91" t="s">
-        <v>442</v>
-      </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="92" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="3" s="52" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="52" t="s">
-        <v>444</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>445</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>401</v>
-      </c>
-      <c r="AMJ3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>446</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>447</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>457</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="29"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>458</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>459</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>461</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>454</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="79" t="s">
-        <v>417</v>
-      </c>
-      <c r="B4" s="79" t="s">
-        <v>465</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>466</v>
-      </c>
-      <c r="D4" s="88" t="n">
-        <v>34</v>
-      </c>
-      <c r="E4" s="89" t="s">
-        <v>467</v>
-      </c>
-      <c r="F4" s="89" t="s">
-        <v>468</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="J4" s="93" t="s">
-        <v>471</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>267</v>
-      </c>
-    </row>
-  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6829,12 +6829,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="6.63967611336032"/>
   </cols>
@@ -7102,20 +7102,20 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="95" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="95" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="B1" s="95" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="C1" s="95" t="s">
         <v>505</v>
@@ -7124,24 +7124,24 @@
         <v>506</v>
       </c>
       <c r="E1" s="95" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="F1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="92" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="92" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
       <c r="F2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="53" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="53" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>445</v>
+        <v>426</v>
       </c>
       <c r="C3" s="53" t="s">
         <v>507</v>
@@ -7157,10 +7157,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="97" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="B4" s="97" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>405</v>
@@ -7171,10 +7171,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="97" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="B5" s="97" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="D5" s="97" t="s">
         <v>408</v>
@@ -7207,9 +7207,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7301,12 +7301,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
@@ -7657,11 +7657,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -7892,7 +7892,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="39" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>563</v>
@@ -8170,10 +8170,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -8242,8 +8242,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.2024291497976"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -8293,8 +8293,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -8347,7 +8347,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -8467,7 +8467,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
@@ -8638,9 +8638,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -8717,7 +8717,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -9096,9 +9096,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.63967611336032"/>
   </cols>
   <sheetData>
@@ -9176,7 +9176,7 @@
         <v>503</v>
       </c>
       <c r="D4" s="89" t="s">
-        <v>419</v>
+        <v>461</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>628</v>
@@ -9200,7 +9200,7 @@
         <v>503</v>
       </c>
       <c r="D5" s="89" t="s">
-        <v>429</v>
+        <v>471</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>632</v>
@@ -9334,10 +9334,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="63.5222672064777"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="96" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9512,8 +9512,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -9907,8 +9907,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9979,26 +9979,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -10267,18 +10267,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="43.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -10429,17 +10429,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -10582,9 +10582,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -10685,14 +10685,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -10863,12 +10863,12 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="6.42914979757085"/>
   </cols>
   <sheetData>
@@ -10898,7 +10898,7 @@
         <v>777</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10950,10 +10950,10 @@
         <v>785</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D4" s="97" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="E4" s="88"/>
       <c r="F4" s="162" t="s">
@@ -10973,10 +10973,10 @@
         <v>787</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D5" s="97" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="F5" s="162" t="s">
         <v>503</v>
@@ -11003,24 +11003,24 @@
   </sheetPr>
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="12" min="7" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.1902834008097"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="6.63967611336032"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="6.63967611336032"/>
   </cols>
@@ -11060,7 +11060,7 @@
         <v>793</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>794</v>
@@ -11139,7 +11139,7 @@
         <v>793</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>794</v>
@@ -11148,7 +11148,7 @@
         <v>795</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>802</v>
@@ -11174,7 +11174,7 @@
         <v>804</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D4" s="79" t="n">
         <v>1</v>
@@ -11202,10 +11202,10 @@
       </c>
       <c r="P4" s="40"/>
       <c r="Q4" s="0" t="s">
-        <v>416</v>
+        <v>459</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="S4" s="0" t="s">
         <v>809</v>
@@ -11222,7 +11222,7 @@
         <v>812</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D5" s="79" t="n">
         <v>0</v>
@@ -11250,10 +11250,10 @@
       </c>
       <c r="P5" s="40"/>
       <c r="Q5" s="0" t="s">
-        <v>421</v>
+        <v>463</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="S5" s="0" t="s">
         <v>809</v>
@@ -11270,7 +11270,7 @@
         <v>817</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D6" s="79" t="n">
         <v>0</v>
@@ -11298,10 +11298,10 @@
       </c>
       <c r="P6" s="40"/>
       <c r="Q6" s="0" t="s">
-        <v>421</v>
+        <v>463</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="S6" s="0" t="s">
         <v>821</v>
@@ -11318,7 +11318,7 @@
         <v>824</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D7" s="79" t="n">
         <v>1</v>
@@ -11344,7 +11344,7 @@
       </c>
       <c r="P7" s="40"/>
       <c r="R7" s="0" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="S7" s="0" t="s">
         <v>827</v>
@@ -11361,7 +11361,7 @@
         <v>830</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D8" s="79" t="n">
         <v>1</v>
@@ -11387,7 +11387,7 @@
       </c>
       <c r="P8" s="40"/>
       <c r="R8" s="0" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11398,7 +11398,7 @@
         <v>835</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>417</v>
+        <v>446</v>
       </c>
       <c r="D9" s="79" t="n">
         <v>0</v>
@@ -11451,10 +11451,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -11749,7 +11749,7 @@
         <v>889</v>
       </c>
       <c r="C27" s="165" t="s">
-        <v>419</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12185,7 +12185,7 @@
         <v>941</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>418</v>
+        <v>460</v>
       </c>
       <c r="G22" s="51" t="s">
         <v>942</v>
@@ -12211,7 +12211,7 @@
         <v>946</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>422</v>
+        <v>464</v>
       </c>
       <c r="G23" s="51" t="s">
         <v>947</v>
@@ -12243,7 +12243,7 @@
         <v>953</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>424</v>
+        <v>466</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12260,7 +12260,7 @@
         <v>957</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>420</v>
+        <v>462</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13193,8 +13193,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="28" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -13366,12 +13366,12 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="6.42914979757085"/>
   </cols>
   <sheetData>
@@ -13475,8 +13475,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -13573,11 +13573,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="180" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="180" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -15663,7 +15663,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74898785425101"/>
@@ -15905,7 +15905,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
@@ -16064,7 +16064,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.497975708502"/>
@@ -16073,7 +16073,7 @@
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="33.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -16543,13 +16543,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.497975708502"/>
@@ -16912,9 +16912,9 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>